<commit_message>
Petite update du Gantt
Mise à jour des deadlines pour la tâche 1 de l'étape 2 de la phase 1
</commit_message>
<xml_diff>
--- a/Gestion de Projet/Phase 0/Tableau de bord.xlsx
+++ b/Gestion de Projet/Phase 0/Tableau de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\Documents\Chess-3000\Gestion de Projet\Phase 0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057393CD-243A-45B0-97BB-6A16F2BAF2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EA594B-7573-4B69-96E3-3CEEA2B064AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,7 +467,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="194">
   <si>
     <t>WBS</t>
   </si>
@@ -494,9 +494,6 @@
   </si>
   <si>
     <t>[Task]</t>
-  </si>
-  <si>
-    <t>[Name]</t>
   </si>
   <si>
     <t>Changing the Color of the Bars in the Gantt Chart</t>
@@ -3826,30 +3823,30 @@
     <xf numFmtId="0" fontId="87" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="46" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="46" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -4230,14 +4227,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>299830</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>803413</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>186607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>130037</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>63776</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>287498</xdr:rowOff>
     </xdr:to>
@@ -5029,7 +5026,7 @@
   <dimension ref="A1:BN45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -5038,7 +5035,7 @@
     <col min="1" max="1" width="6.88671875" customWidth="1"/>
     <col min="2" max="2" width="25.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="8" width="6.6640625" customWidth="1"/>
@@ -5049,7 +5046,7 @@
   <sheetData>
     <row r="1" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="96" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -5057,33 +5054,33 @@
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="I1" s="102"/>
-      <c r="K1" s="206" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="206"/>
-      <c r="M1" s="206"/>
-      <c r="N1" s="206"/>
-      <c r="O1" s="206"/>
-      <c r="P1" s="206"/>
-      <c r="Q1" s="206"/>
-      <c r="R1" s="206"/>
-      <c r="S1" s="206"/>
-      <c r="T1" s="206"/>
-      <c r="U1" s="206"/>
-      <c r="V1" s="206"/>
-      <c r="W1" s="206"/>
-      <c r="X1" s="206"/>
-      <c r="Y1" s="206"/>
-      <c r="Z1" s="206"/>
-      <c r="AA1" s="206"/>
-      <c r="AB1" s="206"/>
-      <c r="AC1" s="206"/>
-      <c r="AD1" s="206"/>
-      <c r="AE1" s="206"/>
+      <c r="K1" s="212" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="212"/>
+      <c r="M1" s="212"/>
+      <c r="N1" s="212"/>
+      <c r="O1" s="212"/>
+      <c r="P1" s="212"/>
+      <c r="Q1" s="212"/>
+      <c r="R1" s="212"/>
+      <c r="S1" s="212"/>
+      <c r="T1" s="212"/>
+      <c r="U1" s="212"/>
+      <c r="V1" s="212"/>
+      <c r="W1" s="212"/>
+      <c r="X1" s="212"/>
+      <c r="Y1" s="212"/>
+      <c r="Z1" s="212"/>
+      <c r="AA1" s="212"/>
+      <c r="AB1" s="212"/>
+      <c r="AC1" s="212"/>
+      <c r="AD1" s="212"/>
+      <c r="AE1" s="212"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -5117,110 +5114,110 @@
     <row r="4" spans="1:66" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="86"/>
       <c r="B4" s="87" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="210">
+        <v>75</v>
+      </c>
+      <c r="C4" s="213">
         <v>45684</v>
       </c>
-      <c r="D4" s="210"/>
-      <c r="E4" s="210"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="213"/>
       <c r="F4" s="86"/>
       <c r="G4" s="87" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="99">
         <v>2</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="31"/>
-      <c r="K4" s="207" t="str">
+      <c r="K4" s="206" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="L4" s="208"/>
-      <c r="M4" s="208"/>
-      <c r="N4" s="208"/>
-      <c r="O4" s="208"/>
-      <c r="P4" s="208"/>
-      <c r="Q4" s="209"/>
-      <c r="R4" s="207" t="str">
+      <c r="L4" s="207"/>
+      <c r="M4" s="207"/>
+      <c r="N4" s="207"/>
+      <c r="O4" s="207"/>
+      <c r="P4" s="207"/>
+      <c r="Q4" s="208"/>
+      <c r="R4" s="206" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="S4" s="208"/>
-      <c r="T4" s="208"/>
-      <c r="U4" s="208"/>
-      <c r="V4" s="208"/>
-      <c r="W4" s="208"/>
-      <c r="X4" s="209"/>
-      <c r="Y4" s="207" t="str">
+      <c r="S4" s="207"/>
+      <c r="T4" s="207"/>
+      <c r="U4" s="207"/>
+      <c r="V4" s="207"/>
+      <c r="W4" s="207"/>
+      <c r="X4" s="208"/>
+      <c r="Y4" s="206" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="Z4" s="208"/>
-      <c r="AA4" s="208"/>
-      <c r="AB4" s="208"/>
-      <c r="AC4" s="208"/>
-      <c r="AD4" s="208"/>
-      <c r="AE4" s="209"/>
-      <c r="AF4" s="207" t="str">
+      <c r="Z4" s="207"/>
+      <c r="AA4" s="207"/>
+      <c r="AB4" s="207"/>
+      <c r="AC4" s="207"/>
+      <c r="AD4" s="207"/>
+      <c r="AE4" s="208"/>
+      <c r="AF4" s="206" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AG4" s="208"/>
-      <c r="AH4" s="208"/>
-      <c r="AI4" s="208"/>
-      <c r="AJ4" s="208"/>
-      <c r="AK4" s="208"/>
-      <c r="AL4" s="209"/>
-      <c r="AM4" s="207" t="str">
+      <c r="AG4" s="207"/>
+      <c r="AH4" s="207"/>
+      <c r="AI4" s="207"/>
+      <c r="AJ4" s="207"/>
+      <c r="AK4" s="207"/>
+      <c r="AL4" s="208"/>
+      <c r="AM4" s="206" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AN4" s="208"/>
-      <c r="AO4" s="208"/>
-      <c r="AP4" s="208"/>
-      <c r="AQ4" s="208"/>
-      <c r="AR4" s="208"/>
-      <c r="AS4" s="209"/>
-      <c r="AT4" s="207" t="str">
+      <c r="AN4" s="207"/>
+      <c r="AO4" s="207"/>
+      <c r="AP4" s="207"/>
+      <c r="AQ4" s="207"/>
+      <c r="AR4" s="207"/>
+      <c r="AS4" s="208"/>
+      <c r="AT4" s="206" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="AU4" s="208"/>
-      <c r="AV4" s="208"/>
-      <c r="AW4" s="208"/>
-      <c r="AX4" s="208"/>
-      <c r="AY4" s="208"/>
-      <c r="AZ4" s="209"/>
-      <c r="BA4" s="207" t="str">
+      <c r="AU4" s="207"/>
+      <c r="AV4" s="207"/>
+      <c r="AW4" s="207"/>
+      <c r="AX4" s="207"/>
+      <c r="AY4" s="207"/>
+      <c r="AZ4" s="208"/>
+      <c r="BA4" s="206" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BB4" s="208"/>
-      <c r="BC4" s="208"/>
-      <c r="BD4" s="208"/>
-      <c r="BE4" s="208"/>
-      <c r="BF4" s="208"/>
-      <c r="BG4" s="209"/>
-      <c r="BH4" s="207" t="str">
+      <c r="BB4" s="207"/>
+      <c r="BC4" s="207"/>
+      <c r="BD4" s="207"/>
+      <c r="BE4" s="207"/>
+      <c r="BF4" s="207"/>
+      <c r="BG4" s="208"/>
+      <c r="BH4" s="206" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BI4" s="208"/>
-      <c r="BJ4" s="208"/>
-      <c r="BK4" s="208"/>
-      <c r="BL4" s="208"/>
-      <c r="BM4" s="208"/>
-      <c r="BN4" s="209"/>
+      <c r="BI4" s="207"/>
+      <c r="BJ4" s="207"/>
+      <c r="BK4" s="207"/>
+      <c r="BL4" s="207"/>
+      <c r="BM4" s="207"/>
+      <c r="BN4" s="208"/>
     </row>
     <row r="5" spans="1:66" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
       <c r="B5" s="87" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="214" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D5" s="214"/>
       <c r="E5" s="214"/>
@@ -5229,86 +5226,86 @@
       <c r="H5" s="86"/>
       <c r="I5" s="86"/>
       <c r="J5" s="31"/>
-      <c r="K5" s="211">
+      <c r="K5" s="209">
         <f>K6</f>
         <v>45691</v>
       </c>
-      <c r="L5" s="212"/>
-      <c r="M5" s="212"/>
-      <c r="N5" s="212"/>
-      <c r="O5" s="212"/>
-      <c r="P5" s="212"/>
-      <c r="Q5" s="213"/>
-      <c r="R5" s="211">
+      <c r="L5" s="210"/>
+      <c r="M5" s="210"/>
+      <c r="N5" s="210"/>
+      <c r="O5" s="210"/>
+      <c r="P5" s="210"/>
+      <c r="Q5" s="211"/>
+      <c r="R5" s="209">
         <f>R6</f>
         <v>45698</v>
       </c>
-      <c r="S5" s="212"/>
-      <c r="T5" s="212"/>
-      <c r="U5" s="212"/>
-      <c r="V5" s="212"/>
-      <c r="W5" s="212"/>
-      <c r="X5" s="213"/>
-      <c r="Y5" s="211">
+      <c r="S5" s="210"/>
+      <c r="T5" s="210"/>
+      <c r="U5" s="210"/>
+      <c r="V5" s="210"/>
+      <c r="W5" s="210"/>
+      <c r="X5" s="211"/>
+      <c r="Y5" s="209">
         <f>Y6</f>
         <v>45705</v>
       </c>
-      <c r="Z5" s="212"/>
-      <c r="AA5" s="212"/>
-      <c r="AB5" s="212"/>
-      <c r="AC5" s="212"/>
-      <c r="AD5" s="212"/>
-      <c r="AE5" s="213"/>
-      <c r="AF5" s="211">
+      <c r="Z5" s="210"/>
+      <c r="AA5" s="210"/>
+      <c r="AB5" s="210"/>
+      <c r="AC5" s="210"/>
+      <c r="AD5" s="210"/>
+      <c r="AE5" s="211"/>
+      <c r="AF5" s="209">
         <f>AF6</f>
         <v>45712</v>
       </c>
-      <c r="AG5" s="212"/>
-      <c r="AH5" s="212"/>
-      <c r="AI5" s="212"/>
-      <c r="AJ5" s="212"/>
-      <c r="AK5" s="212"/>
-      <c r="AL5" s="213"/>
-      <c r="AM5" s="211">
+      <c r="AG5" s="210"/>
+      <c r="AH5" s="210"/>
+      <c r="AI5" s="210"/>
+      <c r="AJ5" s="210"/>
+      <c r="AK5" s="210"/>
+      <c r="AL5" s="211"/>
+      <c r="AM5" s="209">
         <f>AM6</f>
         <v>45719</v>
       </c>
-      <c r="AN5" s="212"/>
-      <c r="AO5" s="212"/>
-      <c r="AP5" s="212"/>
-      <c r="AQ5" s="212"/>
-      <c r="AR5" s="212"/>
-      <c r="AS5" s="213"/>
-      <c r="AT5" s="211">
+      <c r="AN5" s="210"/>
+      <c r="AO5" s="210"/>
+      <c r="AP5" s="210"/>
+      <c r="AQ5" s="210"/>
+      <c r="AR5" s="210"/>
+      <c r="AS5" s="211"/>
+      <c r="AT5" s="209">
         <f>AT6</f>
         <v>45726</v>
       </c>
-      <c r="AU5" s="212"/>
-      <c r="AV5" s="212"/>
-      <c r="AW5" s="212"/>
-      <c r="AX5" s="212"/>
-      <c r="AY5" s="212"/>
-      <c r="AZ5" s="213"/>
-      <c r="BA5" s="211">
+      <c r="AU5" s="210"/>
+      <c r="AV5" s="210"/>
+      <c r="AW5" s="210"/>
+      <c r="AX5" s="210"/>
+      <c r="AY5" s="210"/>
+      <c r="AZ5" s="211"/>
+      <c r="BA5" s="209">
         <f>BA6</f>
         <v>45733</v>
       </c>
-      <c r="BB5" s="212"/>
-      <c r="BC5" s="212"/>
-      <c r="BD5" s="212"/>
-      <c r="BE5" s="212"/>
-      <c r="BF5" s="212"/>
-      <c r="BG5" s="213"/>
-      <c r="BH5" s="211">
+      <c r="BB5" s="210"/>
+      <c r="BC5" s="210"/>
+      <c r="BD5" s="210"/>
+      <c r="BE5" s="210"/>
+      <c r="BF5" s="210"/>
+      <c r="BG5" s="211"/>
+      <c r="BH5" s="209">
         <f>BH6</f>
         <v>45740</v>
       </c>
-      <c r="BI5" s="212"/>
-      <c r="BJ5" s="212"/>
-      <c r="BK5" s="212"/>
-      <c r="BL5" s="212"/>
-      <c r="BM5" s="212"/>
-      <c r="BN5" s="213"/>
+      <c r="BI5" s="210"/>
+      <c r="BJ5" s="210"/>
+      <c r="BK5" s="210"/>
+      <c r="BL5" s="210"/>
+      <c r="BM5" s="210"/>
+      <c r="BN5" s="211"/>
     </row>
     <row r="6" spans="1:66" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
@@ -5551,28 +5548,28 @@
         <v>0</v>
       </c>
       <c r="B7" s="89" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="90" t="s">
+      <c r="D7" s="91" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="91" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="92" t="s">
+      <c r="F7" s="92" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="92" t="s">
+      <c r="G7" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="90" t="s">
+      <c r="H7" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="90" t="s">
+      <c r="I7" s="90" t="s">
         <v>72</v>
-      </c>
-      <c r="I7" s="90" t="s">
-        <v>73</v>
       </c>
       <c r="J7" s="90"/>
       <c r="K7" s="93" t="str">
@@ -5806,7 +5803,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="63" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C8" s="64"/>
       <c r="D8" s="65"/>
@@ -5885,10 +5882,7 @@
         <v>0.1</v>
       </c>
       <c r="B9" s="97" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>9</v>
+        <v>177</v>
       </c>
       <c r="D9" s="98"/>
       <c r="E9" s="77">
@@ -5972,7 +5966,7 @@
         <v>0.2</v>
       </c>
       <c r="B10" s="97" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D10" s="98"/>
       <c r="E10" s="77">
@@ -6057,7 +6051,7 @@
         <v>0.3</v>
       </c>
       <c r="B11" s="97" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D11" s="98"/>
       <c r="E11" s="77">
@@ -6142,7 +6136,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="79"/>
@@ -6220,14 +6214,14 @@
         <v>1.1</v>
       </c>
       <c r="B13" s="204" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D13" s="98"/>
       <c r="E13" s="77"/>
       <c r="F13" s="78"/>
       <c r="G13" s="42">
         <f>G14+G15+G16</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H13" s="43">
         <v>0</v>
@@ -6300,7 +6294,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="98"/>
       <c r="E14" s="77">
@@ -6384,7 +6378,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B15" s="61" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D15" s="98"/>
       <c r="E15" s="77">
@@ -6469,7 +6463,7 @@
         <v>1.1.3</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D16" s="98"/>
       <c r="E16" s="77">
@@ -6478,17 +6472,17 @@
       </c>
       <c r="F16" s="78">
         <f t="shared" si="6"/>
-        <v>45701</v>
+        <v>45703</v>
       </c>
       <c r="G16" s="42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H16" s="43">
-        <v>0.34</v>
+        <v>1</v>
       </c>
       <c r="I16" s="44">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J16" s="73"/>
       <c r="K16" s="40"/>
@@ -6554,14 +6548,14 @@
         <v>1.2</v>
       </c>
       <c r="B17" s="204" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D17" s="98"/>
       <c r="E17" s="77"/>
       <c r="F17" s="78"/>
       <c r="G17" s="42">
         <f>G18+G19+G20</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H17" s="43">
         <v>0</v>
@@ -6634,26 +6628,26 @@
         <v>1.2.1</v>
       </c>
       <c r="B18" s="61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D18" s="197"/>
       <c r="E18" s="198">
         <f>F16+1</f>
-        <v>45702</v>
+        <v>45704</v>
       </c>
       <c r="F18" s="78">
         <f t="shared" si="6"/>
-        <v>45704</v>
+        <v>45709</v>
       </c>
       <c r="G18" s="200">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H18" s="43">
         <v>0</v>
       </c>
       <c r="I18" s="44">
         <f t="shared" ref="I18:I21" si="7">IF(OR(F18=0,E18=0)," - ",NETWORKDAYS(E18,F18))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J18" s="203"/>
       <c r="K18" s="40"/>
@@ -6719,26 +6713,26 @@
         <v>1.2.2</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D19" s="197"/>
       <c r="E19" s="198">
         <f>F18+1</f>
-        <v>45705</v>
+        <v>45710</v>
       </c>
       <c r="F19" s="78">
         <f t="shared" si="6"/>
-        <v>45710</v>
+        <v>45712</v>
       </c>
       <c r="G19" s="200">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H19" s="43">
         <v>0</v>
       </c>
       <c r="I19" s="44">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J19" s="203"/>
       <c r="K19" s="40"/>
@@ -6804,26 +6798,27 @@
         <v>1.2.3</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D20" s="197"/>
       <c r="E20" s="198">
         <f>E19</f>
-        <v>45705</v>
+        <v>45710</v>
       </c>
       <c r="F20" s="78">
         <f t="shared" si="6"/>
-        <v>45710</v>
+        <v>45712</v>
       </c>
       <c r="G20" s="200">
-        <v>6</v>
+        <f>G19</f>
+        <v>3</v>
       </c>
       <c r="H20" s="43">
         <v>0</v>
       </c>
       <c r="I20" s="44">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J20" s="203"/>
       <c r="K20" s="40"/>
@@ -6889,26 +6884,26 @@
         <v>1.3</v>
       </c>
       <c r="B21" s="204" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D21" s="197"/>
       <c r="E21" s="198">
         <f>F20+1</f>
-        <v>45711</v>
+        <v>45713</v>
       </c>
       <c r="F21" s="78">
         <v>45718</v>
       </c>
       <c r="G21" s="200">
         <f>F21-E21</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H21" s="43">
         <v>0</v>
       </c>
       <c r="I21" s="44">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J21" s="203"/>
       <c r="K21" s="40"/>
@@ -7175,7 +7170,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D25" s="36"/>
       <c r="E25" s="79"/>
@@ -7673,7 +7668,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D31" s="36"/>
       <c r="E31" s="79"/>
@@ -8379,7 +8374,7 @@
     </row>
     <row r="40" spans="1:66" s="50" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A40" s="56" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="57"/>
       <c r="C40" s="57"/>
@@ -8453,7 +8448,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="101" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C41" s="58"/>
       <c r="D41" s="59"/>
@@ -8532,7 +8527,7 @@
         <v>1.1</v>
       </c>
       <c r="B42" s="60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C42" s="60"/>
       <c r="D42" s="59"/>
@@ -8611,7 +8606,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B43" s="61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43" s="60"/>
       <c r="D43" s="59"/>
@@ -8690,7 +8685,7 @@
         <v>1.1.1.1</v>
       </c>
       <c r="B44" s="61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C44" s="60"/>
       <c r="D44" s="59"/>
@@ -8772,6 +8767,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="C5:E6"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -8782,15 +8786,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="C5:E6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="H8:H44">
@@ -8836,7 +8831,7 @@
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
     <ignoredError sqref="H9 A37:B38 B32 B33:B35 B26:B29 A40:B40 B39 E12 E25 E31 E37:H40 G12:H12 G25:H25 G31:H35 G41 G42:G43 G44 H26:H29" unlockedFormula="1"/>
-    <ignoredError sqref="A31 A25 A12" formula="1"/>
+    <ignoredError sqref="A31 A25 A12 E20" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -8924,10 +8919,10 @@
     </row>
     <row r="2" spans="2:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="176" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C2" s="222" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D2" s="222"/>
       <c r="E2" s="222"/>
@@ -8936,19 +8931,19 @@
       <c r="H2" s="222"/>
       <c r="I2" s="178"/>
       <c r="J2" s="217" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K2" s="217"/>
       <c r="L2" s="217"/>
       <c r="N2" s="177" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="176"/>
       <c r="C3" s="170"/>
       <c r="D3" s="169" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E3" s="218" t="str">
         <f>GanttChart!C5</f>
@@ -8960,25 +8955,25 @@
       <c r="G3" s="218"/>
       <c r="H3" s="219"/>
       <c r="I3" s="175" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J3" s="174" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K3" s="173" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L3" s="172" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N3" s="171" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="170"/>
       <c r="D4" s="169" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E4" s="220">
         <f>GanttChart!C4</f>
@@ -9001,26 +8996,26 @@
         <v>0</v>
       </c>
       <c r="N4" s="165" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N5" s="165" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="164"/>
       <c r="C6" s="216" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D6" s="216"/>
       <c r="E6" s="216" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F6" s="216"/>
       <c r="G6" s="216" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H6" s="216"/>
       <c r="I6" s="216"/>
@@ -9028,42 +9023,42 @@
       <c r="K6" s="164"/>
       <c r="L6" s="164"/>
       <c r="N6" s="163" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="159" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" s="162" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D7" s="160" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E7" s="162" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F7" s="160" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G7" s="162" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H7" s="161" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I7" s="160" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J7" s="159" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K7" s="158" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L7" s="157" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M7" s="156"/>
       <c r="N7" s="155"/>
@@ -9094,7 +9089,7 @@
       </c>
       <c r="M8" s="131"/>
       <c r="N8" s="141" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
@@ -9426,7 +9421,7 @@
     </row>
     <row r="22" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B22" s="148" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C22" s="147"/>
       <c r="D22" s="146"/>
@@ -9452,7 +9447,7 @@
     </row>
     <row r="23" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B23" s="140" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C23" s="139"/>
       <c r="D23" s="138"/>
@@ -9475,7 +9470,7 @@
     </row>
     <row r="24" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B24" s="140" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" s="139"/>
       <c r="D24" s="138"/>
@@ -9498,7 +9493,7 @@
     </row>
     <row r="25" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B25" s="140" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C25" s="139"/>
       <c r="D25" s="138"/>
@@ -9521,7 +9516,7 @@
     </row>
     <row r="26" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B26" s="140" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C26" s="139"/>
       <c r="D26" s="138"/>
@@ -9544,7 +9539,7 @@
     </row>
     <row r="27" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B27" s="140" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C27" s="139"/>
       <c r="D27" s="138"/>
@@ -9679,13 +9674,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="26"/>
     </row>
     <row r="2" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="108" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3"/>
     </row>
@@ -9694,28 +9689,28 @@
     </row>
     <row r="4" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="103" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="16"/>
     </row>
     <row r="5" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
       <c r="B5" s="109" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B7" s="109" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B9" s="108" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B11" s="107" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9727,13 +9722,13 @@
     <row r="15" spans="1:3" s="104" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="111"/>
       <c r="B15" s="110" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="104" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A16" s="111"/>
       <c r="B16" s="110" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="106" t="s">
         <v>3</v>
@@ -9742,25 +9737,25 @@
     <row r="17" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="112"/>
       <c r="B17" s="110" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="112"/>
       <c r="B18" s="110" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="112"/>
       <c r="B19" s="110" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="104" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="111"/>
       <c r="B20" s="110" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="105" t="s">
         <v>2</v>
@@ -9769,13 +9764,13 @@
     <row r="21" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="112"/>
       <c r="B21" s="110" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="112"/>
       <c r="B22" s="113" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9784,14 +9779,14 @@
     </row>
     <row r="24" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="223" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="223"/>
     </row>
     <row r="25" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A25" s="112"/>
       <c r="B25" s="110" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9801,19 +9796,19 @@
     <row r="27" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="112"/>
       <c r="B27" s="127" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="112"/>
       <c r="B28" s="110" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="112"/>
       <c r="B29" s="110" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9823,19 +9818,19 @@
     <row r="31" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="112"/>
       <c r="B31" s="127" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="112"/>
       <c r="B32" s="110" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="112"/>
       <c r="B33" s="110" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9845,13 +9840,13 @@
     <row r="35" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A35" s="112"/>
       <c r="B35" s="110" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="112"/>
       <c r="B36" s="114" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9860,28 +9855,28 @@
     </row>
     <row r="38" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="223" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" s="223"/>
     </row>
     <row r="39" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B39" s="110" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B41" s="110" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B43" s="110" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B45" s="110" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -9889,7 +9884,7 @@
     </row>
     <row r="47" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B47" s="110" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9900,91 +9895,91 @@
     </row>
     <row r="50" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B50" s="110" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A52" s="115" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="110" t="s">
         <v>12</v>
-      </c>
-      <c r="B52" s="110" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A53" s="115" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="110" t="s">
         <v>14</v>
-      </c>
-      <c r="B53" s="110" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A54" s="115" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" s="110" t="s">
         <v>16</v>
-      </c>
-      <c r="B54" s="110" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A55" s="107"/>
       <c r="B55" s="110" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A56" s="107"/>
       <c r="B56" s="110" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A57" s="115" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="110" t="s">
         <v>18</v>
-      </c>
-      <c r="B57" s="110" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A58" s="107"/>
       <c r="B58" s="110" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A59" s="107"/>
       <c r="B59" s="110" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A60" s="115" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="110" t="s">
         <v>20</v>
-      </c>
-      <c r="B60" s="110" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A61" s="107"/>
       <c r="B61" s="110" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A62" s="115" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" s="110" t="s">
         <v>110</v>
-      </c>
-      <c r="B62" s="110" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A63" s="116"/>
       <c r="B63" s="110" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -9992,13 +9987,13 @@
     </row>
     <row r="65" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A65" s="223" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B65" s="223"/>
     </row>
     <row r="66" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B66" s="110" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10012,13 +10007,13 @@
         <v>6</v>
       </c>
       <c r="B69" s="123" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A70" s="116"/>
       <c r="B70" s="121" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
@@ -10030,13 +10025,13 @@
         <v>6</v>
       </c>
       <c r="B72" s="123" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A73" s="116"/>
       <c r="B73" s="121" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
@@ -10048,13 +10043,13 @@
         <v>6</v>
       </c>
       <c r="B75" s="125" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A76" s="116"/>
       <c r="B76" s="109" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
@@ -10066,13 +10061,13 @@
         <v>6</v>
       </c>
       <c r="B78" s="125" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A79" s="116"/>
       <c r="B79" s="109" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
@@ -10084,25 +10079,25 @@
         <v>6</v>
       </c>
       <c r="B81" s="125" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A82" s="116"/>
       <c r="B82" s="120" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A83" s="116"/>
       <c r="B83" s="120" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A84" s="116"/>
       <c r="B84" s="120" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
@@ -10114,25 +10109,25 @@
         <v>6</v>
       </c>
       <c r="B86" s="125" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A87" s="116"/>
       <c r="B87" s="109" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A88" s="116"/>
       <c r="B88" s="118" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A89" s="116"/>
       <c r="B89" s="124" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
@@ -10144,18 +10139,18 @@
         <v>6</v>
       </c>
       <c r="B91" s="125" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A92" s="107"/>
       <c r="B92" s="120" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -10198,14 +10193,14 @@
     <row r="1" spans="1:3" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="196"/>
       <c r="B1" s="196" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C1" s="196"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="194"/>
       <c r="B2" s="195" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C2" s="194"/>
     </row>
@@ -10216,14 +10211,14 @@
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B4" s="186" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="183"/>
     </row>
     <row r="5" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A5" s="183"/>
       <c r="B5" s="192" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C5" s="183"/>
     </row>
@@ -10235,14 +10230,14 @@
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="190"/>
       <c r="B7" s="186" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C7" s="189"/>
     </row>
     <row r="8" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A8" s="183"/>
       <c r="B8" s="184" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C8" s="183"/>
     </row>
@@ -10254,14 +10249,14 @@
     <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="190"/>
       <c r="B10" s="186" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C10" s="189"/>
     </row>
     <row r="11" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A11" s="185"/>
       <c r="B11" s="184" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C11" s="183"/>
     </row>
@@ -10273,7 +10268,7 @@
     <row r="13" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A13" s="185"/>
       <c r="B13" s="184" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C13" s="183"/>
     </row>
@@ -10285,14 +10280,14 @@
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" s="185"/>
       <c r="B15" s="186" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C15" s="183"/>
     </row>
     <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A16" s="185"/>
       <c r="B16" s="184" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C16" s="183"/>
     </row>
@@ -10331,7 +10326,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="25"/>
     </row>
@@ -10341,14 +10336,14 @@
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="7"/>
     </row>
@@ -10360,7 +10355,7 @@
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="7"/>
     </row>
@@ -10372,7 +10367,7 @@
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="7"/>
     </row>
@@ -10384,7 +10379,7 @@
     <row r="10" spans="1:3" ht="46.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="7"/>
     </row>
@@ -10396,7 +10391,7 @@
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="7"/>
     </row>
@@ -10408,7 +10403,7 @@
     <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="7"/>
     </row>
@@ -10420,7 +10415,7 @@
     <row r="16" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="7"/>
     </row>
@@ -10432,14 +10427,14 @@
     <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="7"/>
     </row>
@@ -10524,17 +10519,17 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -10542,147 +10537,147 @@
     </row>
     <row r="7" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C7" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C13" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B34" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B39" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B42" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B46" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pré étude des solutions
Vue avec Mathieu, étude de la vidéo et des améliorations possibles, pistes définis pour la phase 2
</commit_message>
<xml_diff>
--- a/Gestion de Projet/Phase 0/Tableau de bord.xlsx
+++ b/Gestion de Projet/Phase 0/Tableau de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\Documents\Chess-3000\Gestion de Projet\Phase 0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EA594B-7573-4B69-96E3-3CEEA2B064AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77DEA0D-16C9-412F-BE7F-521AEB0139E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3823,6 +3823,9 @@
     <xf numFmtId="0" fontId="87" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3831,22 +3834,19 @@
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="46" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="46" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -5026,8 +5026,8 @@
   <dimension ref="A1:BN45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5054,29 +5054,29 @@
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="I1" s="102"/>
-      <c r="K1" s="212" t="s">
+      <c r="K1" s="206" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="212"/>
-      <c r="M1" s="212"/>
-      <c r="N1" s="212"/>
-      <c r="O1" s="212"/>
-      <c r="P1" s="212"/>
-      <c r="Q1" s="212"/>
-      <c r="R1" s="212"/>
-      <c r="S1" s="212"/>
-      <c r="T1" s="212"/>
-      <c r="U1" s="212"/>
-      <c r="V1" s="212"/>
-      <c r="W1" s="212"/>
-      <c r="X1" s="212"/>
-      <c r="Y1" s="212"/>
-      <c r="Z1" s="212"/>
-      <c r="AA1" s="212"/>
-      <c r="AB1" s="212"/>
-      <c r="AC1" s="212"/>
-      <c r="AD1" s="212"/>
-      <c r="AE1" s="212"/>
+      <c r="L1" s="206"/>
+      <c r="M1" s="206"/>
+      <c r="N1" s="206"/>
+      <c r="O1" s="206"/>
+      <c r="P1" s="206"/>
+      <c r="Q1" s="206"/>
+      <c r="R1" s="206"/>
+      <c r="S1" s="206"/>
+      <c r="T1" s="206"/>
+      <c r="U1" s="206"/>
+      <c r="V1" s="206"/>
+      <c r="W1" s="206"/>
+      <c r="X1" s="206"/>
+      <c r="Y1" s="206"/>
+      <c r="Z1" s="206"/>
+      <c r="AA1" s="206"/>
+      <c r="AB1" s="206"/>
+      <c r="AC1" s="206"/>
+      <c r="AD1" s="206"/>
+      <c r="AE1" s="206"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
@@ -5116,11 +5116,11 @@
       <c r="B4" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="213">
+      <c r="C4" s="210">
         <v>45684</v>
       </c>
-      <c r="D4" s="213"/>
-      <c r="E4" s="213"/>
+      <c r="D4" s="210"/>
+      <c r="E4" s="210"/>
       <c r="F4" s="86"/>
       <c r="G4" s="87" t="s">
         <v>74</v>
@@ -5130,86 +5130,86 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="31"/>
-      <c r="K4" s="206" t="str">
+      <c r="K4" s="207" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="L4" s="207"/>
-      <c r="M4" s="207"/>
-      <c r="N4" s="207"/>
-      <c r="O4" s="207"/>
-      <c r="P4" s="207"/>
-      <c r="Q4" s="208"/>
-      <c r="R4" s="206" t="str">
+      <c r="L4" s="208"/>
+      <c r="M4" s="208"/>
+      <c r="N4" s="208"/>
+      <c r="O4" s="208"/>
+      <c r="P4" s="208"/>
+      <c r="Q4" s="209"/>
+      <c r="R4" s="207" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="S4" s="207"/>
-      <c r="T4" s="207"/>
-      <c r="U4" s="207"/>
-      <c r="V4" s="207"/>
-      <c r="W4" s="207"/>
-      <c r="X4" s="208"/>
-      <c r="Y4" s="206" t="str">
+      <c r="S4" s="208"/>
+      <c r="T4" s="208"/>
+      <c r="U4" s="208"/>
+      <c r="V4" s="208"/>
+      <c r="W4" s="208"/>
+      <c r="X4" s="209"/>
+      <c r="Y4" s="207" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="Z4" s="207"/>
-      <c r="AA4" s="207"/>
-      <c r="AB4" s="207"/>
-      <c r="AC4" s="207"/>
-      <c r="AD4" s="207"/>
-      <c r="AE4" s="208"/>
-      <c r="AF4" s="206" t="str">
+      <c r="Z4" s="208"/>
+      <c r="AA4" s="208"/>
+      <c r="AB4" s="208"/>
+      <c r="AC4" s="208"/>
+      <c r="AD4" s="208"/>
+      <c r="AE4" s="209"/>
+      <c r="AF4" s="207" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AG4" s="207"/>
-      <c r="AH4" s="207"/>
-      <c r="AI4" s="207"/>
-      <c r="AJ4" s="207"/>
-      <c r="AK4" s="207"/>
-      <c r="AL4" s="208"/>
-      <c r="AM4" s="206" t="str">
+      <c r="AG4" s="208"/>
+      <c r="AH4" s="208"/>
+      <c r="AI4" s="208"/>
+      <c r="AJ4" s="208"/>
+      <c r="AK4" s="208"/>
+      <c r="AL4" s="209"/>
+      <c r="AM4" s="207" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AN4" s="207"/>
-      <c r="AO4" s="207"/>
-      <c r="AP4" s="207"/>
-      <c r="AQ4" s="207"/>
-      <c r="AR4" s="207"/>
-      <c r="AS4" s="208"/>
-      <c r="AT4" s="206" t="str">
+      <c r="AN4" s="208"/>
+      <c r="AO4" s="208"/>
+      <c r="AP4" s="208"/>
+      <c r="AQ4" s="208"/>
+      <c r="AR4" s="208"/>
+      <c r="AS4" s="209"/>
+      <c r="AT4" s="207" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="AU4" s="207"/>
-      <c r="AV4" s="207"/>
-      <c r="AW4" s="207"/>
-      <c r="AX4" s="207"/>
-      <c r="AY4" s="207"/>
-      <c r="AZ4" s="208"/>
-      <c r="BA4" s="206" t="str">
+      <c r="AU4" s="208"/>
+      <c r="AV4" s="208"/>
+      <c r="AW4" s="208"/>
+      <c r="AX4" s="208"/>
+      <c r="AY4" s="208"/>
+      <c r="AZ4" s="209"/>
+      <c r="BA4" s="207" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BB4" s="207"/>
-      <c r="BC4" s="207"/>
-      <c r="BD4" s="207"/>
-      <c r="BE4" s="207"/>
-      <c r="BF4" s="207"/>
-      <c r="BG4" s="208"/>
-      <c r="BH4" s="206" t="str">
+      <c r="BB4" s="208"/>
+      <c r="BC4" s="208"/>
+      <c r="BD4" s="208"/>
+      <c r="BE4" s="208"/>
+      <c r="BF4" s="208"/>
+      <c r="BG4" s="209"/>
+      <c r="BH4" s="207" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BI4" s="207"/>
-      <c r="BJ4" s="207"/>
-      <c r="BK4" s="207"/>
-      <c r="BL4" s="207"/>
-      <c r="BM4" s="207"/>
-      <c r="BN4" s="208"/>
+      <c r="BI4" s="208"/>
+      <c r="BJ4" s="208"/>
+      <c r="BK4" s="208"/>
+      <c r="BL4" s="208"/>
+      <c r="BM4" s="208"/>
+      <c r="BN4" s="209"/>
     </row>
     <row r="5" spans="1:66" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
@@ -5226,86 +5226,86 @@
       <c r="H5" s="86"/>
       <c r="I5" s="86"/>
       <c r="J5" s="31"/>
-      <c r="K5" s="209">
+      <c r="K5" s="211">
         <f>K6</f>
         <v>45691</v>
       </c>
-      <c r="L5" s="210"/>
-      <c r="M5" s="210"/>
-      <c r="N5" s="210"/>
-      <c r="O5" s="210"/>
-      <c r="P5" s="210"/>
-      <c r="Q5" s="211"/>
-      <c r="R5" s="209">
+      <c r="L5" s="212"/>
+      <c r="M5" s="212"/>
+      <c r="N5" s="212"/>
+      <c r="O5" s="212"/>
+      <c r="P5" s="212"/>
+      <c r="Q5" s="213"/>
+      <c r="R5" s="211">
         <f>R6</f>
         <v>45698</v>
       </c>
-      <c r="S5" s="210"/>
-      <c r="T5" s="210"/>
-      <c r="U5" s="210"/>
-      <c r="V5" s="210"/>
-      <c r="W5" s="210"/>
-      <c r="X5" s="211"/>
-      <c r="Y5" s="209">
+      <c r="S5" s="212"/>
+      <c r="T5" s="212"/>
+      <c r="U5" s="212"/>
+      <c r="V5" s="212"/>
+      <c r="W5" s="212"/>
+      <c r="X5" s="213"/>
+      <c r="Y5" s="211">
         <f>Y6</f>
         <v>45705</v>
       </c>
-      <c r="Z5" s="210"/>
-      <c r="AA5" s="210"/>
-      <c r="AB5" s="210"/>
-      <c r="AC5" s="210"/>
-      <c r="AD5" s="210"/>
-      <c r="AE5" s="211"/>
-      <c r="AF5" s="209">
+      <c r="Z5" s="212"/>
+      <c r="AA5" s="212"/>
+      <c r="AB5" s="212"/>
+      <c r="AC5" s="212"/>
+      <c r="AD5" s="212"/>
+      <c r="AE5" s="213"/>
+      <c r="AF5" s="211">
         <f>AF6</f>
         <v>45712</v>
       </c>
-      <c r="AG5" s="210"/>
-      <c r="AH5" s="210"/>
-      <c r="AI5" s="210"/>
-      <c r="AJ5" s="210"/>
-      <c r="AK5" s="210"/>
-      <c r="AL5" s="211"/>
-      <c r="AM5" s="209">
+      <c r="AG5" s="212"/>
+      <c r="AH5" s="212"/>
+      <c r="AI5" s="212"/>
+      <c r="AJ5" s="212"/>
+      <c r="AK5" s="212"/>
+      <c r="AL5" s="213"/>
+      <c r="AM5" s="211">
         <f>AM6</f>
         <v>45719</v>
       </c>
-      <c r="AN5" s="210"/>
-      <c r="AO5" s="210"/>
-      <c r="AP5" s="210"/>
-      <c r="AQ5" s="210"/>
-      <c r="AR5" s="210"/>
-      <c r="AS5" s="211"/>
-      <c r="AT5" s="209">
+      <c r="AN5" s="212"/>
+      <c r="AO5" s="212"/>
+      <c r="AP5" s="212"/>
+      <c r="AQ5" s="212"/>
+      <c r="AR5" s="212"/>
+      <c r="AS5" s="213"/>
+      <c r="AT5" s="211">
         <f>AT6</f>
         <v>45726</v>
       </c>
-      <c r="AU5" s="210"/>
-      <c r="AV5" s="210"/>
-      <c r="AW5" s="210"/>
-      <c r="AX5" s="210"/>
-      <c r="AY5" s="210"/>
-      <c r="AZ5" s="211"/>
-      <c r="BA5" s="209">
+      <c r="AU5" s="212"/>
+      <c r="AV5" s="212"/>
+      <c r="AW5" s="212"/>
+      <c r="AX5" s="212"/>
+      <c r="AY5" s="212"/>
+      <c r="AZ5" s="213"/>
+      <c r="BA5" s="211">
         <f>BA6</f>
         <v>45733</v>
       </c>
-      <c r="BB5" s="210"/>
-      <c r="BC5" s="210"/>
-      <c r="BD5" s="210"/>
-      <c r="BE5" s="210"/>
-      <c r="BF5" s="210"/>
-      <c r="BG5" s="211"/>
-      <c r="BH5" s="209">
+      <c r="BB5" s="212"/>
+      <c r="BC5" s="212"/>
+      <c r="BD5" s="212"/>
+      <c r="BE5" s="212"/>
+      <c r="BF5" s="212"/>
+      <c r="BG5" s="213"/>
+      <c r="BH5" s="211">
         <f>BH6</f>
         <v>45740</v>
       </c>
-      <c r="BI5" s="210"/>
-      <c r="BJ5" s="210"/>
-      <c r="BK5" s="210"/>
-      <c r="BL5" s="210"/>
-      <c r="BM5" s="210"/>
-      <c r="BN5" s="211"/>
+      <c r="BI5" s="212"/>
+      <c r="BJ5" s="212"/>
+      <c r="BK5" s="212"/>
+      <c r="BL5" s="212"/>
+      <c r="BM5" s="212"/>
+      <c r="BN5" s="213"/>
     </row>
     <row r="6" spans="1:66" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
@@ -6555,7 +6555,7 @@
       <c r="F17" s="78"/>
       <c r="G17" s="42">
         <f>G18+G19+G20</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H17" s="43">
         <v>0</v>
@@ -6632,22 +6632,22 @@
       </c>
       <c r="D18" s="197"/>
       <c r="E18" s="198">
-        <f>F16+1</f>
-        <v>45704</v>
+        <f>F16+7</f>
+        <v>45710</v>
       </c>
       <c r="F18" s="78">
         <f t="shared" si="6"/>
-        <v>45709</v>
+        <v>45710</v>
       </c>
       <c r="G18" s="200">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H18" s="43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="44">
         <f t="shared" ref="I18:I21" si="7">IF(OR(F18=0,E18=0)," - ",NETWORKDAYS(E18,F18))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J18" s="203"/>
       <c r="K18" s="40"/>
@@ -6718,14 +6718,14 @@
       <c r="D19" s="197"/>
       <c r="E19" s="198">
         <f>F18+1</f>
-        <v>45710</v>
+        <v>45711</v>
       </c>
       <c r="F19" s="78">
         <f t="shared" si="6"/>
         <v>45712</v>
       </c>
       <c r="G19" s="200">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H19" s="43">
         <v>0</v>
@@ -6803,7 +6803,7 @@
       <c r="D20" s="197"/>
       <c r="E20" s="198">
         <f>E19</f>
-        <v>45710</v>
+        <v>45711</v>
       </c>
       <c r="F20" s="78">
         <f t="shared" si="6"/>
@@ -6811,7 +6811,7 @@
       </c>
       <c r="G20" s="200">
         <f>G19</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20" s="43">
         <v>0</v>
@@ -8767,15 +8767,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="C5:E6"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -8786,6 +8777,15 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="C5:E6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="H8:H44">

</xml_diff>

<commit_message>
Avancée de la revue
Partie 01 et 02 finie, plus que 03,04,05 et 06
</commit_message>
<xml_diff>
--- a/Gestion de Projet/Phase 0/Tableau de bord.xlsx
+++ b/Gestion de Projet/Phase 0/Tableau de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\Documents\Chess-3000\Gestion de Projet\Phase 0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDCDE23-6BEF-4839-902E-378C9EBF7075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD76D176-7282-431F-ADB1-0778DD06901F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3310,7 +3310,7 @@
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="231">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3874,6 +3874,15 @@
     <xf numFmtId="0" fontId="87" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3882,23 +3891,20 @@
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="46" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="46" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
@@ -3930,33 +3936,6 @@
     </xf>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="48" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="48" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -4298,7 +4277,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="5"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="10"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4311,8 +4290,8 @@
       <xdr:rowOff>186607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>143289</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114714</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>628</xdr:rowOff>
     </xdr:to>
@@ -5104,8 +5083,8 @@
   <dimension ref="A1:BN56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="7" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5115,7 +5094,7 @@
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.88671875" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
     <col min="8" max="8" width="6.6640625" customWidth="1"/>
     <col min="9" max="9" width="6.44140625" customWidth="1"/>
     <col min="10" max="10" width="1.88671875" customWidth="1"/>
@@ -5132,29 +5111,29 @@
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="I1" s="102"/>
-      <c r="K1" s="210" t="s">
+      <c r="K1" s="206" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
-      <c r="P1" s="210"/>
-      <c r="Q1" s="210"/>
-      <c r="R1" s="210"/>
-      <c r="S1" s="210"/>
-      <c r="T1" s="210"/>
-      <c r="U1" s="210"/>
-      <c r="V1" s="210"/>
-      <c r="W1" s="210"/>
-      <c r="X1" s="210"/>
-      <c r="Y1" s="210"/>
-      <c r="Z1" s="210"/>
-      <c r="AA1" s="210"/>
-      <c r="AB1" s="210"/>
-      <c r="AC1" s="210"/>
-      <c r="AD1" s="210"/>
-      <c r="AE1" s="210"/>
+      <c r="L1" s="206"/>
+      <c r="M1" s="206"/>
+      <c r="N1" s="206"/>
+      <c r="O1" s="206"/>
+      <c r="P1" s="206"/>
+      <c r="Q1" s="206"/>
+      <c r="R1" s="206"/>
+      <c r="S1" s="206"/>
+      <c r="T1" s="206"/>
+      <c r="U1" s="206"/>
+      <c r="V1" s="206"/>
+      <c r="W1" s="206"/>
+      <c r="X1" s="206"/>
+      <c r="Y1" s="206"/>
+      <c r="Z1" s="206"/>
+      <c r="AA1" s="206"/>
+      <c r="AB1" s="206"/>
+      <c r="AC1" s="206"/>
+      <c r="AD1" s="206"/>
+      <c r="AE1" s="206"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
@@ -5194,431 +5173,431 @@
       <c r="B4" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="211">
+      <c r="C4" s="210">
         <v>45684</v>
       </c>
-      <c r="D4" s="211"/>
-      <c r="E4" s="211"/>
+      <c r="D4" s="210"/>
+      <c r="E4" s="210"/>
       <c r="F4" s="86"/>
       <c r="G4" s="87" t="s">
         <v>73</v>
       </c>
       <c r="H4" s="99">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="31"/>
-      <c r="K4" s="204" t="str">
+      <c r="K4" s="207" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 5</v>
-      </c>
-      <c r="L4" s="205"/>
-      <c r="M4" s="205"/>
-      <c r="N4" s="205"/>
-      <c r="O4" s="205"/>
-      <c r="P4" s="205"/>
-      <c r="Q4" s="206"/>
-      <c r="R4" s="204" t="str">
+        <v>Week 10</v>
+      </c>
+      <c r="L4" s="208"/>
+      <c r="M4" s="208"/>
+      <c r="N4" s="208"/>
+      <c r="O4" s="208"/>
+      <c r="P4" s="208"/>
+      <c r="Q4" s="209"/>
+      <c r="R4" s="207" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 6</v>
-      </c>
-      <c r="S4" s="205"/>
-      <c r="T4" s="205"/>
-      <c r="U4" s="205"/>
-      <c r="V4" s="205"/>
-      <c r="W4" s="205"/>
-      <c r="X4" s="206"/>
-      <c r="Y4" s="204" t="str">
+        <v>Week 11</v>
+      </c>
+      <c r="S4" s="208"/>
+      <c r="T4" s="208"/>
+      <c r="U4" s="208"/>
+      <c r="V4" s="208"/>
+      <c r="W4" s="208"/>
+      <c r="X4" s="209"/>
+      <c r="Y4" s="207" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 7</v>
-      </c>
-      <c r="Z4" s="205"/>
-      <c r="AA4" s="205"/>
-      <c r="AB4" s="205"/>
-      <c r="AC4" s="205"/>
-      <c r="AD4" s="205"/>
-      <c r="AE4" s="206"/>
-      <c r="AF4" s="204" t="str">
+        <v>Week 12</v>
+      </c>
+      <c r="Z4" s="208"/>
+      <c r="AA4" s="208"/>
+      <c r="AB4" s="208"/>
+      <c r="AC4" s="208"/>
+      <c r="AD4" s="208"/>
+      <c r="AE4" s="209"/>
+      <c r="AF4" s="207" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 8</v>
-      </c>
-      <c r="AG4" s="205"/>
-      <c r="AH4" s="205"/>
-      <c r="AI4" s="205"/>
-      <c r="AJ4" s="205"/>
-      <c r="AK4" s="205"/>
-      <c r="AL4" s="206"/>
-      <c r="AM4" s="204" t="str">
+        <v>Week 13</v>
+      </c>
+      <c r="AG4" s="208"/>
+      <c r="AH4" s="208"/>
+      <c r="AI4" s="208"/>
+      <c r="AJ4" s="208"/>
+      <c r="AK4" s="208"/>
+      <c r="AL4" s="209"/>
+      <c r="AM4" s="207" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 9</v>
-      </c>
-      <c r="AN4" s="205"/>
-      <c r="AO4" s="205"/>
-      <c r="AP4" s="205"/>
-      <c r="AQ4" s="205"/>
-      <c r="AR4" s="205"/>
-      <c r="AS4" s="206"/>
-      <c r="AT4" s="204" t="str">
+        <v>Week 14</v>
+      </c>
+      <c r="AN4" s="208"/>
+      <c r="AO4" s="208"/>
+      <c r="AP4" s="208"/>
+      <c r="AQ4" s="208"/>
+      <c r="AR4" s="208"/>
+      <c r="AS4" s="209"/>
+      <c r="AT4" s="207" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 10</v>
-      </c>
-      <c r="AU4" s="205"/>
-      <c r="AV4" s="205"/>
-      <c r="AW4" s="205"/>
-      <c r="AX4" s="205"/>
-      <c r="AY4" s="205"/>
-      <c r="AZ4" s="206"/>
-      <c r="BA4" s="204" t="str">
+        <v>Week 15</v>
+      </c>
+      <c r="AU4" s="208"/>
+      <c r="AV4" s="208"/>
+      <c r="AW4" s="208"/>
+      <c r="AX4" s="208"/>
+      <c r="AY4" s="208"/>
+      <c r="AZ4" s="209"/>
+      <c r="BA4" s="207" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 11</v>
-      </c>
-      <c r="BB4" s="205"/>
-      <c r="BC4" s="205"/>
-      <c r="BD4" s="205"/>
-      <c r="BE4" s="205"/>
-      <c r="BF4" s="205"/>
-      <c r="BG4" s="206"/>
-      <c r="BH4" s="204" t="str">
+        <v>Week 16</v>
+      </c>
+      <c r="BB4" s="208"/>
+      <c r="BC4" s="208"/>
+      <c r="BD4" s="208"/>
+      <c r="BE4" s="208"/>
+      <c r="BF4" s="208"/>
+      <c r="BG4" s="209"/>
+      <c r="BH4" s="207" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 12</v>
-      </c>
-      <c r="BI4" s="205"/>
-      <c r="BJ4" s="205"/>
-      <c r="BK4" s="205"/>
-      <c r="BL4" s="205"/>
-      <c r="BM4" s="205"/>
-      <c r="BN4" s="206"/>
+        <v>Week 17</v>
+      </c>
+      <c r="BI4" s="208"/>
+      <c r="BJ4" s="208"/>
+      <c r="BK4" s="208"/>
+      <c r="BL4" s="208"/>
+      <c r="BM4" s="208"/>
+      <c r="BN4" s="209"/>
     </row>
     <row r="5" spans="1:66" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
       <c r="B5" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="212" t="s">
+      <c r="C5" s="214" t="s">
         <v>181</v>
       </c>
-      <c r="D5" s="212"/>
-      <c r="E5" s="212"/>
+      <c r="D5" s="214"/>
+      <c r="E5" s="214"/>
       <c r="F5" s="86"/>
       <c r="G5" s="86"/>
       <c r="H5" s="86"/>
       <c r="I5" s="86"/>
       <c r="J5" s="31"/>
-      <c r="K5" s="207">
+      <c r="K5" s="211">
         <f>K6</f>
-        <v>45712</v>
-      </c>
-      <c r="L5" s="208"/>
-      <c r="M5" s="208"/>
-      <c r="N5" s="208"/>
-      <c r="O5" s="208"/>
-      <c r="P5" s="208"/>
-      <c r="Q5" s="209"/>
-      <c r="R5" s="207">
+        <v>45747</v>
+      </c>
+      <c r="L5" s="212"/>
+      <c r="M5" s="212"/>
+      <c r="N5" s="212"/>
+      <c r="O5" s="212"/>
+      <c r="P5" s="212"/>
+      <c r="Q5" s="213"/>
+      <c r="R5" s="211">
         <f>R6</f>
-        <v>45719</v>
-      </c>
-      <c r="S5" s="208"/>
-      <c r="T5" s="208"/>
-      <c r="U5" s="208"/>
-      <c r="V5" s="208"/>
-      <c r="W5" s="208"/>
-      <c r="X5" s="209"/>
-      <c r="Y5" s="207">
+        <v>45754</v>
+      </c>
+      <c r="S5" s="212"/>
+      <c r="T5" s="212"/>
+      <c r="U5" s="212"/>
+      <c r="V5" s="212"/>
+      <c r="W5" s="212"/>
+      <c r="X5" s="213"/>
+      <c r="Y5" s="211">
         <f>Y6</f>
-        <v>45726</v>
-      </c>
-      <c r="Z5" s="208"/>
-      <c r="AA5" s="208"/>
-      <c r="AB5" s="208"/>
-      <c r="AC5" s="208"/>
-      <c r="AD5" s="208"/>
-      <c r="AE5" s="209"/>
-      <c r="AF5" s="207">
+        <v>45761</v>
+      </c>
+      <c r="Z5" s="212"/>
+      <c r="AA5" s="212"/>
+      <c r="AB5" s="212"/>
+      <c r="AC5" s="212"/>
+      <c r="AD5" s="212"/>
+      <c r="AE5" s="213"/>
+      <c r="AF5" s="211">
         <f>AF6</f>
-        <v>45733</v>
-      </c>
-      <c r="AG5" s="208"/>
-      <c r="AH5" s="208"/>
-      <c r="AI5" s="208"/>
-      <c r="AJ5" s="208"/>
-      <c r="AK5" s="208"/>
-      <c r="AL5" s="209"/>
-      <c r="AM5" s="207">
+        <v>45768</v>
+      </c>
+      <c r="AG5" s="212"/>
+      <c r="AH5" s="212"/>
+      <c r="AI5" s="212"/>
+      <c r="AJ5" s="212"/>
+      <c r="AK5" s="212"/>
+      <c r="AL5" s="213"/>
+      <c r="AM5" s="211">
         <f>AM6</f>
-        <v>45740</v>
-      </c>
-      <c r="AN5" s="208"/>
-      <c r="AO5" s="208"/>
-      <c r="AP5" s="208"/>
-      <c r="AQ5" s="208"/>
-      <c r="AR5" s="208"/>
-      <c r="AS5" s="209"/>
-      <c r="AT5" s="207">
+        <v>45775</v>
+      </c>
+      <c r="AN5" s="212"/>
+      <c r="AO5" s="212"/>
+      <c r="AP5" s="212"/>
+      <c r="AQ5" s="212"/>
+      <c r="AR5" s="212"/>
+      <c r="AS5" s="213"/>
+      <c r="AT5" s="211">
         <f>AT6</f>
-        <v>45747</v>
-      </c>
-      <c r="AU5" s="208"/>
-      <c r="AV5" s="208"/>
-      <c r="AW5" s="208"/>
-      <c r="AX5" s="208"/>
-      <c r="AY5" s="208"/>
-      <c r="AZ5" s="209"/>
-      <c r="BA5" s="207">
+        <v>45782</v>
+      </c>
+      <c r="AU5" s="212"/>
+      <c r="AV5" s="212"/>
+      <c r="AW5" s="212"/>
+      <c r="AX5" s="212"/>
+      <c r="AY5" s="212"/>
+      <c r="AZ5" s="213"/>
+      <c r="BA5" s="211">
         <f>BA6</f>
-        <v>45754</v>
-      </c>
-      <c r="BB5" s="208"/>
-      <c r="BC5" s="208"/>
-      <c r="BD5" s="208"/>
-      <c r="BE5" s="208"/>
-      <c r="BF5" s="208"/>
-      <c r="BG5" s="209"/>
-      <c r="BH5" s="207">
+        <v>45789</v>
+      </c>
+      <c r="BB5" s="212"/>
+      <c r="BC5" s="212"/>
+      <c r="BD5" s="212"/>
+      <c r="BE5" s="212"/>
+      <c r="BF5" s="212"/>
+      <c r="BG5" s="213"/>
+      <c r="BH5" s="211">
         <f>BH6</f>
-        <v>45761</v>
-      </c>
-      <c r="BI5" s="208"/>
-      <c r="BJ5" s="208"/>
-      <c r="BK5" s="208"/>
-      <c r="BL5" s="208"/>
-      <c r="BM5" s="208"/>
-      <c r="BN5" s="209"/>
+        <v>45796</v>
+      </c>
+      <c r="BI5" s="212"/>
+      <c r="BJ5" s="212"/>
+      <c r="BK5" s="212"/>
+      <c r="BL5" s="212"/>
+      <c r="BM5" s="212"/>
+      <c r="BN5" s="213"/>
     </row>
     <row r="6" spans="1:66" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="31"/>
-      <c r="C6" s="213"/>
-      <c r="D6" s="213"/>
-      <c r="E6" s="213"/>
+      <c r="C6" s="215"/>
+      <c r="D6" s="215"/>
+      <c r="E6" s="215"/>
       <c r="F6" s="31"/>
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
       <c r="I6" s="31"/>
       <c r="J6" s="31"/>
-      <c r="K6" s="228">
+      <c r="K6" s="70">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>45712</v>
-      </c>
-      <c r="L6" s="229">
+        <v>45747</v>
+      </c>
+      <c r="L6" s="62">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>45713</v>
-      </c>
-      <c r="M6" s="229">
+        <v>45748</v>
+      </c>
+      <c r="M6" s="62">
         <f t="shared" si="0"/>
-        <v>45714</v>
-      </c>
-      <c r="N6" s="229">
+        <v>45749</v>
+      </c>
+      <c r="N6" s="62">
         <f t="shared" si="0"/>
-        <v>45715</v>
-      </c>
-      <c r="O6" s="229">
+        <v>45750</v>
+      </c>
+      <c r="O6" s="62">
         <f t="shared" si="0"/>
-        <v>45716</v>
-      </c>
-      <c r="P6" s="229">
+        <v>45751</v>
+      </c>
+      <c r="P6" s="62">
         <f t="shared" si="0"/>
-        <v>45717</v>
-      </c>
-      <c r="Q6" s="230">
+        <v>45752</v>
+      </c>
+      <c r="Q6" s="71">
         <f t="shared" si="0"/>
-        <v>45718</v>
-      </c>
-      <c r="R6" s="228">
+        <v>45753</v>
+      </c>
+      <c r="R6" s="70">
         <f t="shared" si="0"/>
-        <v>45719</v>
-      </c>
-      <c r="S6" s="229">
+        <v>45754</v>
+      </c>
+      <c r="S6" s="62">
         <f t="shared" si="0"/>
-        <v>45720</v>
-      </c>
-      <c r="T6" s="229">
+        <v>45755</v>
+      </c>
+      <c r="T6" s="62">
         <f t="shared" si="0"/>
-        <v>45721</v>
-      </c>
-      <c r="U6" s="229">
+        <v>45756</v>
+      </c>
+      <c r="U6" s="62">
         <f t="shared" si="0"/>
-        <v>45722</v>
-      </c>
-      <c r="V6" s="229">
+        <v>45757</v>
+      </c>
+      <c r="V6" s="62">
         <f t="shared" si="0"/>
-        <v>45723</v>
-      </c>
-      <c r="W6" s="229">
+        <v>45758</v>
+      </c>
+      <c r="W6" s="62">
         <f t="shared" si="0"/>
-        <v>45724</v>
-      </c>
-      <c r="X6" s="230">
+        <v>45759</v>
+      </c>
+      <c r="X6" s="71">
         <f t="shared" si="0"/>
-        <v>45725</v>
-      </c>
-      <c r="Y6" s="228">
+        <v>45760</v>
+      </c>
+      <c r="Y6" s="70">
         <f t="shared" si="0"/>
-        <v>45726</v>
-      </c>
-      <c r="Z6" s="229">
+        <v>45761</v>
+      </c>
+      <c r="Z6" s="62">
         <f t="shared" si="0"/>
-        <v>45727</v>
-      </c>
-      <c r="AA6" s="229">
+        <v>45762</v>
+      </c>
+      <c r="AA6" s="62">
         <f t="shared" si="0"/>
-        <v>45728</v>
-      </c>
-      <c r="AB6" s="229">
+        <v>45763</v>
+      </c>
+      <c r="AB6" s="62">
         <f t="shared" si="0"/>
-        <v>45729</v>
-      </c>
-      <c r="AC6" s="229">
+        <v>45764</v>
+      </c>
+      <c r="AC6" s="62">
         <f t="shared" si="0"/>
-        <v>45730</v>
-      </c>
-      <c r="AD6" s="229">
+        <v>45765</v>
+      </c>
+      <c r="AD6" s="62">
         <f t="shared" si="0"/>
-        <v>45731</v>
-      </c>
-      <c r="AE6" s="230">
+        <v>45766</v>
+      </c>
+      <c r="AE6" s="71">
         <f t="shared" si="0"/>
-        <v>45732</v>
-      </c>
-      <c r="AF6" s="228">
+        <v>45767</v>
+      </c>
+      <c r="AF6" s="70">
         <f t="shared" si="0"/>
-        <v>45733</v>
-      </c>
-      <c r="AG6" s="229">
+        <v>45768</v>
+      </c>
+      <c r="AG6" s="62">
         <f t="shared" si="0"/>
-        <v>45734</v>
-      </c>
-      <c r="AH6" s="229">
+        <v>45769</v>
+      </c>
+      <c r="AH6" s="62">
         <f t="shared" si="0"/>
-        <v>45735</v>
-      </c>
-      <c r="AI6" s="229">
+        <v>45770</v>
+      </c>
+      <c r="AI6" s="62">
         <f t="shared" si="0"/>
-        <v>45736</v>
-      </c>
-      <c r="AJ6" s="229">
+        <v>45771</v>
+      </c>
+      <c r="AJ6" s="62">
         <f t="shared" si="0"/>
-        <v>45737</v>
-      </c>
-      <c r="AK6" s="229">
+        <v>45772</v>
+      </c>
+      <c r="AK6" s="62">
         <f t="shared" si="0"/>
-        <v>45738</v>
-      </c>
-      <c r="AL6" s="230">
+        <v>45773</v>
+      </c>
+      <c r="AL6" s="71">
         <f t="shared" si="0"/>
-        <v>45739</v>
+        <v>45774</v>
       </c>
       <c r="AM6" s="70">
         <f t="shared" si="0"/>
-        <v>45740</v>
+        <v>45775</v>
       </c>
       <c r="AN6" s="62">
         <f t="shared" si="0"/>
-        <v>45741</v>
+        <v>45776</v>
       </c>
       <c r="AO6" s="62">
         <f t="shared" si="0"/>
-        <v>45742</v>
+        <v>45777</v>
       </c>
       <c r="AP6" s="62">
         <f t="shared" si="0"/>
-        <v>45743</v>
+        <v>45778</v>
       </c>
       <c r="AQ6" s="62">
         <f t="shared" si="0"/>
-        <v>45744</v>
+        <v>45779</v>
       </c>
       <c r="AR6" s="62">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>45745</v>
+        <v>45780</v>
       </c>
       <c r="AS6" s="71">
         <f t="shared" si="1"/>
-        <v>45746</v>
+        <v>45781</v>
       </c>
       <c r="AT6" s="70">
         <f t="shared" si="1"/>
-        <v>45747</v>
+        <v>45782</v>
       </c>
       <c r="AU6" s="62">
         <f t="shared" si="1"/>
-        <v>45748</v>
+        <v>45783</v>
       </c>
       <c r="AV6" s="62">
         <f t="shared" si="1"/>
-        <v>45749</v>
+        <v>45784</v>
       </c>
       <c r="AW6" s="62">
         <f t="shared" si="1"/>
-        <v>45750</v>
+        <v>45785</v>
       </c>
       <c r="AX6" s="62">
         <f t="shared" si="1"/>
-        <v>45751</v>
+        <v>45786</v>
       </c>
       <c r="AY6" s="62">
         <f t="shared" si="1"/>
-        <v>45752</v>
+        <v>45787</v>
       </c>
       <c r="AZ6" s="71">
         <f t="shared" si="1"/>
-        <v>45753</v>
+        <v>45788</v>
       </c>
       <c r="BA6" s="70">
         <f t="shared" si="1"/>
-        <v>45754</v>
+        <v>45789</v>
       </c>
       <c r="BB6" s="62">
         <f t="shared" si="1"/>
-        <v>45755</v>
+        <v>45790</v>
       </c>
       <c r="BC6" s="62">
         <f t="shared" si="1"/>
-        <v>45756</v>
+        <v>45791</v>
       </c>
       <c r="BD6" s="62">
         <f t="shared" si="1"/>
-        <v>45757</v>
+        <v>45792</v>
       </c>
       <c r="BE6" s="62">
         <f t="shared" si="1"/>
-        <v>45758</v>
+        <v>45793</v>
       </c>
       <c r="BF6" s="62">
         <f t="shared" si="1"/>
-        <v>45759</v>
+        <v>45794</v>
       </c>
       <c r="BG6" s="71">
         <f t="shared" si="1"/>
-        <v>45760</v>
+        <v>45795</v>
       </c>
       <c r="BH6" s="70">
         <f t="shared" si="1"/>
-        <v>45761</v>
+        <v>45796</v>
       </c>
       <c r="BI6" s="62">
         <f t="shared" si="1"/>
-        <v>45762</v>
+        <v>45797</v>
       </c>
       <c r="BJ6" s="62">
         <f t="shared" si="1"/>
-        <v>45763</v>
+        <v>45798</v>
       </c>
       <c r="BK6" s="62">
         <f t="shared" si="1"/>
-        <v>45764</v>
+        <v>45799</v>
       </c>
       <c r="BL6" s="62">
         <f t="shared" si="1"/>
-        <v>45765</v>
+        <v>45800</v>
       </c>
       <c r="BM6" s="62">
         <f t="shared" si="1"/>
-        <v>45766</v>
+        <v>45801</v>
       </c>
       <c r="BN6" s="71">
         <f t="shared" si="1"/>
-        <v>45767</v>
+        <v>45802</v>
       </c>
     </row>
     <row r="7" spans="1:66" s="2" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
@@ -6052,7 +6031,7 @@
         <v>45692</v>
       </c>
       <c r="F10" s="78">
-        <f t="shared" ref="F10:F47" si="6">IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
+        <f t="shared" ref="F10:G47" si="6">IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
         <v>45695</v>
       </c>
       <c r="G10" s="42">
@@ -6960,18 +6939,18 @@
         <v>45713</v>
       </c>
       <c r="F21" s="78">
-        <v>45718</v>
-      </c>
-      <c r="G21" s="199">
-        <f>F21-E21</f>
-        <v>5</v>
+        <v>45720</v>
+      </c>
+      <c r="G21" s="42">
+        <f>IF(ISBLANK(F21)," - ",F21-E21+1)</f>
+        <v>8</v>
       </c>
       <c r="H21" s="43">
         <v>0</v>
       </c>
       <c r="I21" s="44">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J21" s="201"/>
       <c r="K21" s="40"/>
@@ -7195,11 +7174,11 @@
       <c r="D24" s="98"/>
       <c r="E24" s="77">
         <f>F21+1</f>
-        <v>45719</v>
+        <v>45721</v>
       </c>
       <c r="F24" s="78">
         <f t="shared" si="6"/>
-        <v>45719</v>
+        <v>45721</v>
       </c>
       <c r="G24" s="42">
         <v>1</v>
@@ -7280,11 +7259,11 @@
       <c r="D25" s="98"/>
       <c r="E25" s="77">
         <f>F24+1</f>
-        <v>45720</v>
+        <v>45722</v>
       </c>
       <c r="F25" s="78">
         <f t="shared" si="6"/>
-        <v>45720</v>
+        <v>45722</v>
       </c>
       <c r="G25" s="42">
         <v>1</v>
@@ -7365,11 +7344,11 @@
       <c r="D26" s="98"/>
       <c r="E26" s="77">
         <f>F25+1</f>
-        <v>45721</v>
+        <v>45723</v>
       </c>
       <c r="F26" s="78">
         <f t="shared" si="6"/>
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="G26" s="42">
         <v>22</v>
@@ -7450,22 +7429,22 @@
       <c r="D27" s="98"/>
       <c r="E27" s="77">
         <f>E26+3</f>
-        <v>45724</v>
+        <v>45726</v>
       </c>
       <c r="F27" s="78">
         <f>F26</f>
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="G27" s="42">
-        <f>F27-E27</f>
-        <v>18</v>
+        <f>IF(ISBLANK(F27)," - ",F27-E27+1)</f>
+        <v>19</v>
       </c>
       <c r="H27" s="43">
         <v>0</v>
       </c>
       <c r="I27" s="44">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J27" s="73"/>
       <c r="K27" s="40"/>
@@ -7536,11 +7515,11 @@
       <c r="D28" s="98"/>
       <c r="E28" s="77">
         <f>F27+1</f>
-        <v>45743</v>
+        <v>45745</v>
       </c>
       <c r="F28" s="78">
         <f t="shared" si="6"/>
-        <v>45745</v>
+        <v>45747</v>
       </c>
       <c r="G28" s="42">
         <v>3</v>
@@ -7550,7 +7529,7 @@
       </c>
       <c r="I28" s="44">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J28" s="73"/>
       <c r="K28" s="40"/>
@@ -7618,16 +7597,16 @@
       <c r="B29" s="202" t="s">
         <v>196</v>
       </c>
-      <c r="D29" s="222"/>
-      <c r="E29" s="223"/>
-      <c r="F29" s="224"/>
-      <c r="G29" s="225"/>
+      <c r="D29" s="197"/>
+      <c r="E29" s="198"/>
+      <c r="F29" s="204"/>
+      <c r="G29" s="199"/>
       <c r="H29" s="200"/>
       <c r="I29" s="44" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J29" s="227"/>
+      <c r="J29" s="201"/>
       <c r="K29" s="40"/>
       <c r="L29" s="40"/>
       <c r="M29" s="40"/>
@@ -7687,22 +7666,22 @@
     </row>
     <row r="30" spans="1:66" s="41" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f t="shared" ref="A30:A36" si="8">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>2.2.1</v>
       </c>
       <c r="B30" s="97" t="s">
         <v>197</v>
       </c>
-      <c r="D30" s="222"/>
-      <c r="E30" s="223">
+      <c r="D30" s="197"/>
+      <c r="E30" s="198">
         <f>F28+1</f>
-        <v>45746</v>
+        <v>45748</v>
       </c>
       <c r="F30" s="78">
         <f t="shared" si="6"/>
-        <v>45746</v>
-      </c>
-      <c r="G30" s="225">
+        <v>45748</v>
+      </c>
+      <c r="G30" s="199">
         <v>1</v>
       </c>
       <c r="H30" s="200">
@@ -7710,9 +7689,9 @@
       </c>
       <c r="I30" s="44">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J30" s="227"/>
+        <v>1</v>
+      </c>
+      <c r="J30" s="201"/>
       <c r="K30" s="40"/>
       <c r="L30" s="40"/>
       <c r="M30" s="40"/>
@@ -7772,22 +7751,22 @@
     </row>
     <row r="31" spans="1:66" s="41" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f t="shared" si="8"/>
         <v>2.2.2</v>
       </c>
       <c r="B31" s="97" t="s">
         <v>192</v>
       </c>
-      <c r="D31" s="222"/>
-      <c r="E31" s="223">
+      <c r="D31" s="197"/>
+      <c r="E31" s="198">
         <f>F30+1</f>
-        <v>45747</v>
+        <v>45749</v>
       </c>
       <c r="F31" s="78">
         <f t="shared" si="6"/>
-        <v>45747</v>
-      </c>
-      <c r="G31" s="225">
+        <v>45749</v>
+      </c>
+      <c r="G31" s="199">
         <v>1</v>
       </c>
       <c r="H31" s="200">
@@ -7797,7 +7776,7 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="J31" s="227"/>
+      <c r="J31" s="201"/>
       <c r="K31" s="40"/>
       <c r="L31" s="40"/>
       <c r="M31" s="40"/>
@@ -7857,22 +7836,22 @@
     </row>
     <row r="32" spans="1:66" s="41" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f t="shared" si="8"/>
         <v>2.2.3</v>
       </c>
       <c r="B32" s="97" t="s">
         <v>193</v>
       </c>
-      <c r="D32" s="222"/>
-      <c r="E32" s="223">
+      <c r="D32" s="197"/>
+      <c r="E32" s="198">
         <f>F31+1</f>
-        <v>45748</v>
+        <v>45750</v>
       </c>
       <c r="F32" s="78">
         <f t="shared" si="6"/>
-        <v>45769</v>
-      </c>
-      <c r="G32" s="225">
+        <v>45771</v>
+      </c>
+      <c r="G32" s="199">
         <v>22</v>
       </c>
       <c r="H32" s="200">
@@ -7882,7 +7861,7 @@
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="J32" s="227"/>
+      <c r="J32" s="201"/>
       <c r="K32" s="40"/>
       <c r="L32" s="40"/>
       <c r="M32" s="40"/>
@@ -7942,33 +7921,33 @@
     </row>
     <row r="33" spans="1:66" s="41" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f t="shared" si="8"/>
         <v>2.2.4</v>
       </c>
       <c r="B33" s="97" t="s">
         <v>198</v>
       </c>
-      <c r="D33" s="222"/>
-      <c r="E33" s="223">
+      <c r="D33" s="197"/>
+      <c r="E33" s="198">
         <f>E32+5</f>
-        <v>45753</v>
-      </c>
-      <c r="F33" s="224">
+        <v>45755</v>
+      </c>
+      <c r="F33" s="204">
         <f>F32</f>
-        <v>45769</v>
-      </c>
-      <c r="G33" s="225">
-        <f>F33-E33</f>
-        <v>16</v>
+        <v>45771</v>
+      </c>
+      <c r="G33" s="42">
+        <f>IF(ISBLANK(F33)," - ",F33-E33+1)</f>
+        <v>17</v>
       </c>
       <c r="H33" s="200">
         <v>0</v>
       </c>
-      <c r="I33" s="226">
+      <c r="I33" s="205">
         <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="J33" s="227"/>
+        <v>13</v>
+      </c>
+      <c r="J33" s="201"/>
       <c r="K33" s="40"/>
       <c r="L33" s="40"/>
       <c r="M33" s="40"/>
@@ -8028,32 +8007,32 @@
     </row>
     <row r="34" spans="1:66" s="41" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f t="shared" si="8"/>
         <v>2.2.5</v>
       </c>
       <c r="B34" s="97" t="s">
         <v>199</v>
       </c>
-      <c r="D34" s="222"/>
-      <c r="E34" s="223">
+      <c r="D34" s="197"/>
+      <c r="E34" s="198">
         <f>F33+1</f>
-        <v>45770</v>
+        <v>45772</v>
       </c>
       <c r="F34" s="78">
         <f t="shared" si="6"/>
-        <v>45772</v>
-      </c>
-      <c r="G34" s="225">
+        <v>45774</v>
+      </c>
+      <c r="G34" s="199">
         <v>3</v>
       </c>
       <c r="H34" s="200">
         <v>0</v>
       </c>
-      <c r="I34" s="226">
+      <c r="I34" s="205">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="J34" s="227"/>
+        <v>1</v>
+      </c>
+      <c r="J34" s="201"/>
       <c r="K34" s="40"/>
       <c r="L34" s="40"/>
       <c r="M34" s="40"/>
@@ -8113,32 +8092,32 @@
     </row>
     <row r="35" spans="1:66" s="41" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f t="shared" si="8"/>
         <v>2.2.6</v>
       </c>
       <c r="B35" s="97" t="s">
         <v>200</v>
       </c>
-      <c r="D35" s="222"/>
-      <c r="E35" s="223">
+      <c r="D35" s="197"/>
+      <c r="E35" s="198">
         <f>F34+1</f>
-        <v>45773</v>
+        <v>45775</v>
       </c>
       <c r="F35" s="78">
         <f t="shared" si="6"/>
-        <v>45773</v>
-      </c>
-      <c r="G35" s="225">
+        <v>45775</v>
+      </c>
+      <c r="G35" s="199">
         <v>1</v>
       </c>
       <c r="H35" s="200">
         <v>0</v>
       </c>
-      <c r="I35" s="226">
+      <c r="I35" s="205">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="227"/>
+        <v>1</v>
+      </c>
+      <c r="J35" s="201"/>
       <c r="K35" s="40"/>
       <c r="L35" s="40"/>
       <c r="M35" s="40"/>
@@ -8198,32 +8177,32 @@
     </row>
     <row r="36" spans="1:66" s="41" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f t="shared" si="8"/>
         <v>2.2.7</v>
       </c>
       <c r="B36" s="97" t="s">
         <v>201</v>
       </c>
-      <c r="D36" s="222"/>
-      <c r="E36" s="223">
+      <c r="D36" s="197"/>
+      <c r="E36" s="198">
         <f>F35+1</f>
-        <v>45774</v>
+        <v>45776</v>
       </c>
       <c r="F36" s="78">
         <f t="shared" si="6"/>
-        <v>45776</v>
-      </c>
-      <c r="G36" s="225">
+        <v>45778</v>
+      </c>
+      <c r="G36" s="199">
         <v>3</v>
       </c>
       <c r="H36" s="200">
         <v>0</v>
       </c>
-      <c r="I36" s="226">
+      <c r="I36" s="205">
         <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="J36" s="227"/>
+        <v>3</v>
+      </c>
+      <c r="J36" s="201"/>
       <c r="K36" s="40"/>
       <c r="L36" s="40"/>
       <c r="M36" s="40"/>
@@ -8289,26 +8268,26 @@
       <c r="B37" s="202" t="s">
         <v>202</v>
       </c>
-      <c r="D37" s="222"/>
-      <c r="E37" s="223">
+      <c r="D37" s="197"/>
+      <c r="E37" s="198">
         <f>F36+1</f>
-        <v>45777</v>
+        <v>45779</v>
       </c>
       <c r="F37" s="78">
         <f t="shared" si="6"/>
-        <v>45781</v>
-      </c>
-      <c r="G37" s="225">
+        <v>45783</v>
+      </c>
+      <c r="G37" s="199">
         <v>5</v>
       </c>
       <c r="H37" s="200">
         <v>0</v>
       </c>
-      <c r="I37" s="226">
+      <c r="I37" s="205">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="J37" s="227"/>
+      <c r="J37" s="201"/>
       <c r="K37" s="40"/>
       <c r="L37" s="40"/>
       <c r="M37" s="40"/>
@@ -8374,16 +8353,16 @@
       <c r="B38" s="202" t="s">
         <v>204</v>
       </c>
-      <c r="D38" s="222"/>
-      <c r="E38" s="223"/>
+      <c r="D38" s="197"/>
+      <c r="E38" s="198"/>
       <c r="F38" s="78"/>
-      <c r="G38" s="225"/>
+      <c r="G38" s="199"/>
       <c r="H38" s="200"/>
-      <c r="I38" s="226" t="str">
+      <c r="I38" s="205" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J38" s="227"/>
+      <c r="J38" s="201"/>
       <c r="K38" s="40"/>
       <c r="L38" s="40"/>
       <c r="M38" s="40"/>
@@ -8449,26 +8428,26 @@
       <c r="B39" s="97" t="s">
         <v>205</v>
       </c>
-      <c r="D39" s="222"/>
-      <c r="E39" s="223">
+      <c r="D39" s="197"/>
+      <c r="E39" s="198">
         <f>F37+1</f>
-        <v>45782</v>
+        <v>45784</v>
       </c>
       <c r="F39" s="78">
         <f t="shared" si="6"/>
-        <v>45801</v>
-      </c>
-      <c r="G39" s="225">
+        <v>45803</v>
+      </c>
+      <c r="G39" s="199">
         <v>20</v>
       </c>
       <c r="H39" s="200">
         <v>0</v>
       </c>
-      <c r="I39" s="226">
+      <c r="I39" s="205">
         <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="J39" s="227"/>
+        <v>14</v>
+      </c>
+      <c r="J39" s="201"/>
       <c r="K39" s="40"/>
       <c r="L39" s="40"/>
       <c r="M39" s="40"/>
@@ -8534,26 +8513,26 @@
       <c r="B40" s="97" t="s">
         <v>199</v>
       </c>
-      <c r="D40" s="222"/>
-      <c r="E40" s="223">
+      <c r="D40" s="197"/>
+      <c r="E40" s="198">
         <f>F39+1</f>
-        <v>45802</v>
+        <v>45804</v>
       </c>
       <c r="F40" s="78">
         <f t="shared" si="6"/>
-        <v>45806</v>
-      </c>
-      <c r="G40" s="225">
+        <v>45808</v>
+      </c>
+      <c r="G40" s="199">
         <v>5</v>
       </c>
       <c r="H40" s="200">
         <v>0</v>
       </c>
-      <c r="I40" s="226">
+      <c r="I40" s="205">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="J40" s="227"/>
+      <c r="J40" s="201"/>
       <c r="K40" s="40"/>
       <c r="L40" s="40"/>
       <c r="M40" s="40"/>
@@ -8619,26 +8598,26 @@
       <c r="B41" s="97" t="s">
         <v>206</v>
       </c>
-      <c r="D41" s="222"/>
-      <c r="E41" s="223">
+      <c r="D41" s="197"/>
+      <c r="E41" s="198">
         <f>F40+1</f>
-        <v>45807</v>
+        <v>45809</v>
       </c>
       <c r="F41" s="78">
         <f t="shared" si="6"/>
-        <v>45811</v>
-      </c>
-      <c r="G41" s="225">
+        <v>45813</v>
+      </c>
+      <c r="G41" s="199">
         <v>5</v>
       </c>
       <c r="H41" s="200">
         <v>0</v>
       </c>
-      <c r="I41" s="226">
+      <c r="I41" s="205">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="J41" s="227"/>
+        <v>4</v>
+      </c>
+      <c r="J41" s="201"/>
       <c r="K41" s="40"/>
       <c r="L41" s="40"/>
       <c r="M41" s="40"/>
@@ -8860,11 +8839,11 @@
       <c r="D44" s="98"/>
       <c r="E44" s="77">
         <f>F41+1</f>
-        <v>45812</v>
+        <v>45814</v>
       </c>
       <c r="F44" s="78">
         <f t="shared" si="6"/>
-        <v>45821</v>
+        <v>45823</v>
       </c>
       <c r="G44" s="42">
         <v>10</v>
@@ -8874,7 +8853,7 @@
       </c>
       <c r="I44" s="44">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J44" s="73"/>
       <c r="K44" s="40"/>
@@ -8945,11 +8924,11 @@
       <c r="D45" s="98"/>
       <c r="E45" s="77">
         <f>F44+1</f>
-        <v>45822</v>
+        <v>45824</v>
       </c>
       <c r="F45" s="78">
         <f t="shared" si="6"/>
-        <v>45826</v>
+        <v>45828</v>
       </c>
       <c r="G45" s="42">
         <v>5</v>
@@ -8959,7 +8938,7 @@
       </c>
       <c r="I45" s="44">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J45" s="73"/>
       <c r="K45" s="40"/>
@@ -9030,11 +9009,11 @@
       <c r="D46" s="98"/>
       <c r="E46" s="77">
         <f>E45</f>
-        <v>45822</v>
+        <v>45824</v>
       </c>
       <c r="F46" s="78">
         <f t="shared" si="6"/>
-        <v>45826</v>
+        <v>45828</v>
       </c>
       <c r="G46" s="42">
         <v>5</v>
@@ -9044,7 +9023,7 @@
       </c>
       <c r="I46" s="44">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J46" s="73"/>
       <c r="K46" s="40"/>
@@ -9114,22 +9093,23 @@
       </c>
       <c r="D47" s="98"/>
       <c r="E47" s="77">
-        <f>F46+1</f>
-        <v>45827</v>
+        <f>E46+2</f>
+        <v>45826</v>
       </c>
       <c r="F47" s="78">
-        <f t="shared" si="6"/>
+        <f>F46</f>
         <v>45828</v>
       </c>
       <c r="G47" s="42">
-        <v>2</v>
+        <f>IF(ISBLANK(F47)," - ",F47-E47+1)</f>
+        <v>3</v>
       </c>
       <c r="H47" s="43">
         <v>0</v>
       </c>
       <c r="I47" s="44">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J47" s="73"/>
       <c r="K47" s="40"/>
@@ -9482,7 +9462,7 @@
       <c r="D52" s="59"/>
       <c r="E52" s="77"/>
       <c r="F52" s="78" t="str">
-        <f t="shared" ref="F52:F55" si="8">IF(ISBLANK(E52)," - ",IF(G52=0,E52,E52+G52-1))</f>
+        <f t="shared" ref="F52:F55" si="9">IF(ISBLANK(E52)," - ",IF(G52=0,E52,E52+G52-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G52" s="42"/>
@@ -9561,13 +9541,13 @@
       <c r="D53" s="59"/>
       <c r="E53" s="77"/>
       <c r="F53" s="78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G53" s="42"/>
       <c r="H53" s="43"/>
       <c r="I53" s="44" t="str">
-        <f t="shared" ref="I53:I55" si="9">IF(OR(F53=0,E53=0)," - ",NETWORKDAYS(E53,F53))</f>
+        <f t="shared" ref="I53:I55" si="10">IF(OR(F53=0,E53=0)," - ",NETWORKDAYS(E53,F53))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J53" s="73"/>
@@ -9640,13 +9620,13 @@
       <c r="D54" s="59"/>
       <c r="E54" s="77"/>
       <c r="F54" s="78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G54" s="42"/>
       <c r="H54" s="43"/>
       <c r="I54" s="44" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J54" s="73"/>
@@ -9719,13 +9699,13 @@
       <c r="D55" s="59"/>
       <c r="E55" s="77"/>
       <c r="F55" s="78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G55" s="42"/>
       <c r="H55" s="43"/>
       <c r="I55" s="44" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J55" s="73"/>
@@ -9795,15 +9775,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="C5:E6"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -9814,6 +9785,15 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="C5:E6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="H8:H55">
@@ -9848,7 +9828,7 @@
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Project Start Date." sqref="H4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <hyperlinks>
@@ -9949,20 +9929,20 @@
       <c r="B2" s="176" t="s">
         <v>161</v>
       </c>
-      <c r="C2" s="220" t="s">
+      <c r="C2" s="222" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="220"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
       <c r="I2" s="178"/>
-      <c r="J2" s="215" t="s">
+      <c r="J2" s="217" t="s">
         <v>159</v>
       </c>
-      <c r="K2" s="215"/>
-      <c r="L2" s="215"/>
+      <c r="K2" s="217"/>
+      <c r="L2" s="217"/>
       <c r="N2" s="177" t="s">
         <v>158</v>
       </c>
@@ -9973,15 +9953,15 @@
       <c r="D3" s="169" t="s">
         <v>157</v>
       </c>
-      <c r="E3" s="216" t="str">
+      <c r="E3" s="218" t="str">
         <f>GanttChart!C5</f>
         <v>Laurentin Turcat, 
 Mathis Pradelles, 
 Mathieu Anziani</v>
       </c>
-      <c r="F3" s="216"/>
-      <c r="G3" s="216"/>
-      <c r="H3" s="217"/>
+      <c r="F3" s="218"/>
+      <c r="G3" s="218"/>
+      <c r="H3" s="219"/>
       <c r="I3" s="175" t="s">
         <v>156</v>
       </c>
@@ -10003,13 +9983,13 @@
       <c r="D4" s="169" t="s">
         <v>154</v>
       </c>
-      <c r="E4" s="218">
+      <c r="E4" s="220">
         <f>GanttChart!C4</f>
         <v>45684</v>
       </c>
-      <c r="F4" s="218"/>
-      <c r="G4" s="218"/>
-      <c r="H4" s="219"/>
+      <c r="F4" s="220"/>
+      <c r="G4" s="220"/>
+      <c r="H4" s="221"/>
       <c r="I4" s="168"/>
       <c r="J4" s="166">
         <f>SUBTOTAL(9,J7:J185)</f>
@@ -10034,19 +10014,19 @@
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="164"/>
-      <c r="C6" s="214" t="s">
+      <c r="C6" s="216" t="s">
         <v>151</v>
       </c>
-      <c r="D6" s="214"/>
-      <c r="E6" s="214" t="s">
+      <c r="D6" s="216"/>
+      <c r="E6" s="216" t="s">
         <v>150</v>
       </c>
-      <c r="F6" s="214"/>
-      <c r="G6" s="214" t="s">
+      <c r="F6" s="216"/>
+      <c r="G6" s="216" t="s">
         <v>149</v>
       </c>
-      <c r="H6" s="214"/>
-      <c r="I6" s="214"/>
+      <c r="H6" s="216"/>
+      <c r="I6" s="216"/>
       <c r="J6" s="164"/>
       <c r="K6" s="164"/>
       <c r="L6" s="164"/>
@@ -11183,10 +11163,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A13" s="221" t="s">
+      <c r="A13" s="223" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="221"/>
+      <c r="B13" s="223"/>
     </row>
     <row r="15" spans="1:3" s="104" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="111"/>
@@ -11247,10 +11227,10 @@
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="221" t="s">
+      <c r="A24" s="223" t="s">
         <v>85</v>
       </c>
-      <c r="B24" s="221"/>
+      <c r="B24" s="223"/>
     </row>
     <row r="25" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A25" s="112"/>
@@ -11323,10 +11303,10 @@
       <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A38" s="221" t="s">
+      <c r="A38" s="223" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="221"/>
+      <c r="B38" s="223"/>
     </row>
     <row r="39" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B39" s="110" t="s">
@@ -11357,10 +11337,10 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="221" t="s">
+      <c r="A49" s="223" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="221"/>
+      <c r="B49" s="223"/>
     </row>
     <row r="50" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B50" s="110" t="s">
@@ -11455,10 +11435,10 @@
       <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="221" t="s">
+      <c r="A65" s="223" t="s">
         <v>8</v>
       </c>
-      <c r="B65" s="221"/>
+      <c r="B65" s="223"/>
     </row>
     <row r="66" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B66" s="110" t="s">
@@ -11466,10 +11446,10 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="221" t="s">
+      <c r="A68" s="223" t="s">
         <v>5</v>
       </c>
-      <c r="B68" s="221"/>
+      <c r="B68" s="223"/>
     </row>
     <row r="69" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A69" s="122" t="s">

</xml_diff>

<commit_message>
Grosse avancée sur la revue
Partie 3, 4 et 5 terminée
</commit_message>
<xml_diff>
--- a/Gestion de Projet/Phase 0/Tableau de bord.xlsx
+++ b/Gestion de Projet/Phase 0/Tableau de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\Documents\Chess-3000\Gestion de Projet\Phase 0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD76D176-7282-431F-ADB1-0778DD06901F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9309EF70-7C23-4231-BDF7-B5564B9E88BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3880,30 +3880,30 @@
     <xf numFmtId="1" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="46" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="46" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -4277,7 +4277,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="5"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5082,9 +5082,9 @@
   </sheetPr>
   <dimension ref="A1:BN56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J45" sqref="J45"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BO16" sqref="BO16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5111,29 +5111,29 @@
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="I1" s="102"/>
-      <c r="K1" s="206" t="s">
+      <c r="K1" s="212" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="206"/>
-      <c r="M1" s="206"/>
-      <c r="N1" s="206"/>
-      <c r="O1" s="206"/>
-      <c r="P1" s="206"/>
-      <c r="Q1" s="206"/>
-      <c r="R1" s="206"/>
-      <c r="S1" s="206"/>
-      <c r="T1" s="206"/>
-      <c r="U1" s="206"/>
-      <c r="V1" s="206"/>
-      <c r="W1" s="206"/>
-      <c r="X1" s="206"/>
-      <c r="Y1" s="206"/>
-      <c r="Z1" s="206"/>
-      <c r="AA1" s="206"/>
-      <c r="AB1" s="206"/>
-      <c r="AC1" s="206"/>
-      <c r="AD1" s="206"/>
-      <c r="AE1" s="206"/>
+      <c r="L1" s="212"/>
+      <c r="M1" s="212"/>
+      <c r="N1" s="212"/>
+      <c r="O1" s="212"/>
+      <c r="P1" s="212"/>
+      <c r="Q1" s="212"/>
+      <c r="R1" s="212"/>
+      <c r="S1" s="212"/>
+      <c r="T1" s="212"/>
+      <c r="U1" s="212"/>
+      <c r="V1" s="212"/>
+      <c r="W1" s="212"/>
+      <c r="X1" s="212"/>
+      <c r="Y1" s="212"/>
+      <c r="Z1" s="212"/>
+      <c r="AA1" s="212"/>
+      <c r="AB1" s="212"/>
+      <c r="AC1" s="212"/>
+      <c r="AD1" s="212"/>
+      <c r="AE1" s="212"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
@@ -5173,100 +5173,100 @@
       <c r="B4" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="210">
+      <c r="C4" s="213">
         <v>45684</v>
       </c>
-      <c r="D4" s="210"/>
-      <c r="E4" s="210"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="213"/>
       <c r="F4" s="86"/>
       <c r="G4" s="87" t="s">
         <v>73</v>
       </c>
       <c r="H4" s="99">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="31"/>
-      <c r="K4" s="207" t="str">
+      <c r="K4" s="206" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 5</v>
+      </c>
+      <c r="L4" s="207"/>
+      <c r="M4" s="207"/>
+      <c r="N4" s="207"/>
+      <c r="O4" s="207"/>
+      <c r="P4" s="207"/>
+      <c r="Q4" s="208"/>
+      <c r="R4" s="206" t="str">
+        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 6</v>
+      </c>
+      <c r="S4" s="207"/>
+      <c r="T4" s="207"/>
+      <c r="U4" s="207"/>
+      <c r="V4" s="207"/>
+      <c r="W4" s="207"/>
+      <c r="X4" s="208"/>
+      <c r="Y4" s="206" t="str">
+        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 7</v>
+      </c>
+      <c r="Z4" s="207"/>
+      <c r="AA4" s="207"/>
+      <c r="AB4" s="207"/>
+      <c r="AC4" s="207"/>
+      <c r="AD4" s="207"/>
+      <c r="AE4" s="208"/>
+      <c r="AF4" s="206" t="str">
+        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 8</v>
+      </c>
+      <c r="AG4" s="207"/>
+      <c r="AH4" s="207"/>
+      <c r="AI4" s="207"/>
+      <c r="AJ4" s="207"/>
+      <c r="AK4" s="207"/>
+      <c r="AL4" s="208"/>
+      <c r="AM4" s="206" t="str">
+        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 9</v>
+      </c>
+      <c r="AN4" s="207"/>
+      <c r="AO4" s="207"/>
+      <c r="AP4" s="207"/>
+      <c r="AQ4" s="207"/>
+      <c r="AR4" s="207"/>
+      <c r="AS4" s="208"/>
+      <c r="AT4" s="206" t="str">
+        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="L4" s="208"/>
-      <c r="M4" s="208"/>
-      <c r="N4" s="208"/>
-      <c r="O4" s="208"/>
-      <c r="P4" s="208"/>
-      <c r="Q4" s="209"/>
-      <c r="R4" s="207" t="str">
-        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AU4" s="207"/>
+      <c r="AV4" s="207"/>
+      <c r="AW4" s="207"/>
+      <c r="AX4" s="207"/>
+      <c r="AY4" s="207"/>
+      <c r="AZ4" s="208"/>
+      <c r="BA4" s="206" t="str">
+        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="S4" s="208"/>
-      <c r="T4" s="208"/>
-      <c r="U4" s="208"/>
-      <c r="V4" s="208"/>
-      <c r="W4" s="208"/>
-      <c r="X4" s="209"/>
-      <c r="Y4" s="207" t="str">
-        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BB4" s="207"/>
+      <c r="BC4" s="207"/>
+      <c r="BD4" s="207"/>
+      <c r="BE4" s="207"/>
+      <c r="BF4" s="207"/>
+      <c r="BG4" s="208"/>
+      <c r="BH4" s="206" t="str">
+        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="Z4" s="208"/>
-      <c r="AA4" s="208"/>
-      <c r="AB4" s="208"/>
-      <c r="AC4" s="208"/>
-      <c r="AD4" s="208"/>
-      <c r="AE4" s="209"/>
-      <c r="AF4" s="207" t="str">
-        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 13</v>
-      </c>
-      <c r="AG4" s="208"/>
-      <c r="AH4" s="208"/>
-      <c r="AI4" s="208"/>
-      <c r="AJ4" s="208"/>
-      <c r="AK4" s="208"/>
-      <c r="AL4" s="209"/>
-      <c r="AM4" s="207" t="str">
-        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 14</v>
-      </c>
-      <c r="AN4" s="208"/>
-      <c r="AO4" s="208"/>
-      <c r="AP4" s="208"/>
-      <c r="AQ4" s="208"/>
-      <c r="AR4" s="208"/>
-      <c r="AS4" s="209"/>
-      <c r="AT4" s="207" t="str">
-        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 15</v>
-      </c>
-      <c r="AU4" s="208"/>
-      <c r="AV4" s="208"/>
-      <c r="AW4" s="208"/>
-      <c r="AX4" s="208"/>
-      <c r="AY4" s="208"/>
-      <c r="AZ4" s="209"/>
-      <c r="BA4" s="207" t="str">
-        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 16</v>
-      </c>
-      <c r="BB4" s="208"/>
-      <c r="BC4" s="208"/>
-      <c r="BD4" s="208"/>
-      <c r="BE4" s="208"/>
-      <c r="BF4" s="208"/>
-      <c r="BG4" s="209"/>
-      <c r="BH4" s="207" t="str">
-        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 17</v>
-      </c>
-      <c r="BI4" s="208"/>
-      <c r="BJ4" s="208"/>
-      <c r="BK4" s="208"/>
-      <c r="BL4" s="208"/>
-      <c r="BM4" s="208"/>
-      <c r="BN4" s="209"/>
+      <c r="BI4" s="207"/>
+      <c r="BJ4" s="207"/>
+      <c r="BK4" s="207"/>
+      <c r="BL4" s="207"/>
+      <c r="BM4" s="207"/>
+      <c r="BN4" s="208"/>
     </row>
     <row r="5" spans="1:66" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
@@ -5283,86 +5283,86 @@
       <c r="H5" s="86"/>
       <c r="I5" s="86"/>
       <c r="J5" s="31"/>
-      <c r="K5" s="211">
+      <c r="K5" s="209">
         <f>K6</f>
+        <v>45712</v>
+      </c>
+      <c r="L5" s="210"/>
+      <c r="M5" s="210"/>
+      <c r="N5" s="210"/>
+      <c r="O5" s="210"/>
+      <c r="P5" s="210"/>
+      <c r="Q5" s="211"/>
+      <c r="R5" s="209">
+        <f>R6</f>
+        <v>45719</v>
+      </c>
+      <c r="S5" s="210"/>
+      <c r="T5" s="210"/>
+      <c r="U5" s="210"/>
+      <c r="V5" s="210"/>
+      <c r="W5" s="210"/>
+      <c r="X5" s="211"/>
+      <c r="Y5" s="209">
+        <f>Y6</f>
+        <v>45726</v>
+      </c>
+      <c r="Z5" s="210"/>
+      <c r="AA5" s="210"/>
+      <c r="AB5" s="210"/>
+      <c r="AC5" s="210"/>
+      <c r="AD5" s="210"/>
+      <c r="AE5" s="211"/>
+      <c r="AF5" s="209">
+        <f>AF6</f>
+        <v>45733</v>
+      </c>
+      <c r="AG5" s="210"/>
+      <c r="AH5" s="210"/>
+      <c r="AI5" s="210"/>
+      <c r="AJ5" s="210"/>
+      <c r="AK5" s="210"/>
+      <c r="AL5" s="211"/>
+      <c r="AM5" s="209">
+        <f>AM6</f>
+        <v>45740</v>
+      </c>
+      <c r="AN5" s="210"/>
+      <c r="AO5" s="210"/>
+      <c r="AP5" s="210"/>
+      <c r="AQ5" s="210"/>
+      <c r="AR5" s="210"/>
+      <c r="AS5" s="211"/>
+      <c r="AT5" s="209">
+        <f>AT6</f>
         <v>45747</v>
       </c>
-      <c r="L5" s="212"/>
-      <c r="M5" s="212"/>
-      <c r="N5" s="212"/>
-      <c r="O5" s="212"/>
-      <c r="P5" s="212"/>
-      <c r="Q5" s="213"/>
-      <c r="R5" s="211">
-        <f>R6</f>
+      <c r="AU5" s="210"/>
+      <c r="AV5" s="210"/>
+      <c r="AW5" s="210"/>
+      <c r="AX5" s="210"/>
+      <c r="AY5" s="210"/>
+      <c r="AZ5" s="211"/>
+      <c r="BA5" s="209">
+        <f>BA6</f>
         <v>45754</v>
       </c>
-      <c r="S5" s="212"/>
-      <c r="T5" s="212"/>
-      <c r="U5" s="212"/>
-      <c r="V5" s="212"/>
-      <c r="W5" s="212"/>
-      <c r="X5" s="213"/>
-      <c r="Y5" s="211">
-        <f>Y6</f>
+      <c r="BB5" s="210"/>
+      <c r="BC5" s="210"/>
+      <c r="BD5" s="210"/>
+      <c r="BE5" s="210"/>
+      <c r="BF5" s="210"/>
+      <c r="BG5" s="211"/>
+      <c r="BH5" s="209">
+        <f>BH6</f>
         <v>45761</v>
       </c>
-      <c r="Z5" s="212"/>
-      <c r="AA5" s="212"/>
-      <c r="AB5" s="212"/>
-      <c r="AC5" s="212"/>
-      <c r="AD5" s="212"/>
-      <c r="AE5" s="213"/>
-      <c r="AF5" s="211">
-        <f>AF6</f>
-        <v>45768</v>
-      </c>
-      <c r="AG5" s="212"/>
-      <c r="AH5" s="212"/>
-      <c r="AI5" s="212"/>
-      <c r="AJ5" s="212"/>
-      <c r="AK5" s="212"/>
-      <c r="AL5" s="213"/>
-      <c r="AM5" s="211">
-        <f>AM6</f>
-        <v>45775</v>
-      </c>
-      <c r="AN5" s="212"/>
-      <c r="AO5" s="212"/>
-      <c r="AP5" s="212"/>
-      <c r="AQ5" s="212"/>
-      <c r="AR5" s="212"/>
-      <c r="AS5" s="213"/>
-      <c r="AT5" s="211">
-        <f>AT6</f>
-        <v>45782</v>
-      </c>
-      <c r="AU5" s="212"/>
-      <c r="AV5" s="212"/>
-      <c r="AW5" s="212"/>
-      <c r="AX5" s="212"/>
-      <c r="AY5" s="212"/>
-      <c r="AZ5" s="213"/>
-      <c r="BA5" s="211">
-        <f>BA6</f>
-        <v>45789</v>
-      </c>
-      <c r="BB5" s="212"/>
-      <c r="BC5" s="212"/>
-      <c r="BD5" s="212"/>
-      <c r="BE5" s="212"/>
-      <c r="BF5" s="212"/>
-      <c r="BG5" s="213"/>
-      <c r="BH5" s="211">
-        <f>BH6</f>
-        <v>45796</v>
-      </c>
-      <c r="BI5" s="212"/>
-      <c r="BJ5" s="212"/>
-      <c r="BK5" s="212"/>
-      <c r="BL5" s="212"/>
-      <c r="BM5" s="212"/>
-      <c r="BN5" s="213"/>
+      <c r="BI5" s="210"/>
+      <c r="BJ5" s="210"/>
+      <c r="BK5" s="210"/>
+      <c r="BL5" s="210"/>
+      <c r="BM5" s="210"/>
+      <c r="BN5" s="211"/>
     </row>
     <row r="6" spans="1:66" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
@@ -5377,227 +5377,227 @@
       <c r="J6" s="31"/>
       <c r="K6" s="70">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>45747</v>
+        <v>45712</v>
       </c>
       <c r="L6" s="62">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>45748</v>
+        <v>45713</v>
       </c>
       <c r="M6" s="62">
         <f t="shared" si="0"/>
-        <v>45749</v>
+        <v>45714</v>
       </c>
       <c r="N6" s="62">
         <f t="shared" si="0"/>
-        <v>45750</v>
+        <v>45715</v>
       </c>
       <c r="O6" s="62">
         <f t="shared" si="0"/>
-        <v>45751</v>
+        <v>45716</v>
       </c>
       <c r="P6" s="62">
         <f t="shared" si="0"/>
-        <v>45752</v>
+        <v>45717</v>
       </c>
       <c r="Q6" s="71">
         <f t="shared" si="0"/>
-        <v>45753</v>
+        <v>45718</v>
       </c>
       <c r="R6" s="70">
         <f t="shared" si="0"/>
-        <v>45754</v>
+        <v>45719</v>
       </c>
       <c r="S6" s="62">
         <f t="shared" si="0"/>
-        <v>45755</v>
+        <v>45720</v>
       </c>
       <c r="T6" s="62">
         <f t="shared" si="0"/>
-        <v>45756</v>
+        <v>45721</v>
       </c>
       <c r="U6" s="62">
         <f t="shared" si="0"/>
-        <v>45757</v>
+        <v>45722</v>
       </c>
       <c r="V6" s="62">
         <f t="shared" si="0"/>
-        <v>45758</v>
+        <v>45723</v>
       </c>
       <c r="W6" s="62">
         <f t="shared" si="0"/>
-        <v>45759</v>
+        <v>45724</v>
       </c>
       <c r="X6" s="71">
         <f t="shared" si="0"/>
-        <v>45760</v>
+        <v>45725</v>
       </c>
       <c r="Y6" s="70">
         <f t="shared" si="0"/>
-        <v>45761</v>
+        <v>45726</v>
       </c>
       <c r="Z6" s="62">
         <f t="shared" si="0"/>
-        <v>45762</v>
+        <v>45727</v>
       </c>
       <c r="AA6" s="62">
         <f t="shared" si="0"/>
-        <v>45763</v>
+        <v>45728</v>
       </c>
       <c r="AB6" s="62">
         <f t="shared" si="0"/>
-        <v>45764</v>
+        <v>45729</v>
       </c>
       <c r="AC6" s="62">
         <f t="shared" si="0"/>
-        <v>45765</v>
+        <v>45730</v>
       </c>
       <c r="AD6" s="62">
         <f t="shared" si="0"/>
-        <v>45766</v>
+        <v>45731</v>
       </c>
       <c r="AE6" s="71">
         <f t="shared" si="0"/>
-        <v>45767</v>
+        <v>45732</v>
       </c>
       <c r="AF6" s="70">
         <f t="shared" si="0"/>
-        <v>45768</v>
+        <v>45733</v>
       </c>
       <c r="AG6" s="62">
         <f t="shared" si="0"/>
-        <v>45769</v>
+        <v>45734</v>
       </c>
       <c r="AH6" s="62">
         <f t="shared" si="0"/>
-        <v>45770</v>
+        <v>45735</v>
       </c>
       <c r="AI6" s="62">
         <f t="shared" si="0"/>
-        <v>45771</v>
+        <v>45736</v>
       </c>
       <c r="AJ6" s="62">
         <f t="shared" si="0"/>
-        <v>45772</v>
+        <v>45737</v>
       </c>
       <c r="AK6" s="62">
         <f t="shared" si="0"/>
-        <v>45773</v>
+        <v>45738</v>
       </c>
       <c r="AL6" s="71">
         <f t="shared" si="0"/>
-        <v>45774</v>
+        <v>45739</v>
       </c>
       <c r="AM6" s="70">
         <f t="shared" si="0"/>
-        <v>45775</v>
+        <v>45740</v>
       </c>
       <c r="AN6" s="62">
         <f t="shared" si="0"/>
-        <v>45776</v>
+        <v>45741</v>
       </c>
       <c r="AO6" s="62">
         <f t="shared" si="0"/>
-        <v>45777</v>
+        <v>45742</v>
       </c>
       <c r="AP6" s="62">
         <f t="shared" si="0"/>
-        <v>45778</v>
+        <v>45743</v>
       </c>
       <c r="AQ6" s="62">
         <f t="shared" si="0"/>
-        <v>45779</v>
+        <v>45744</v>
       </c>
       <c r="AR6" s="62">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>45780</v>
+        <v>45745</v>
       </c>
       <c r="AS6" s="71">
         <f t="shared" si="1"/>
-        <v>45781</v>
+        <v>45746</v>
       </c>
       <c r="AT6" s="70">
         <f t="shared" si="1"/>
-        <v>45782</v>
+        <v>45747</v>
       </c>
       <c r="AU6" s="62">
         <f t="shared" si="1"/>
-        <v>45783</v>
+        <v>45748</v>
       </c>
       <c r="AV6" s="62">
         <f t="shared" si="1"/>
-        <v>45784</v>
+        <v>45749</v>
       </c>
       <c r="AW6" s="62">
         <f t="shared" si="1"/>
-        <v>45785</v>
+        <v>45750</v>
       </c>
       <c r="AX6" s="62">
         <f t="shared" si="1"/>
-        <v>45786</v>
+        <v>45751</v>
       </c>
       <c r="AY6" s="62">
         <f t="shared" si="1"/>
-        <v>45787</v>
+        <v>45752</v>
       </c>
       <c r="AZ6" s="71">
         <f t="shared" si="1"/>
-        <v>45788</v>
+        <v>45753</v>
       </c>
       <c r="BA6" s="70">
         <f t="shared" si="1"/>
-        <v>45789</v>
+        <v>45754</v>
       </c>
       <c r="BB6" s="62">
         <f t="shared" si="1"/>
-        <v>45790</v>
+        <v>45755</v>
       </c>
       <c r="BC6" s="62">
         <f t="shared" si="1"/>
-        <v>45791</v>
+        <v>45756</v>
       </c>
       <c r="BD6" s="62">
         <f t="shared" si="1"/>
-        <v>45792</v>
+        <v>45757</v>
       </c>
       <c r="BE6" s="62">
         <f t="shared" si="1"/>
-        <v>45793</v>
+        <v>45758</v>
       </c>
       <c r="BF6" s="62">
         <f t="shared" si="1"/>
-        <v>45794</v>
+        <v>45759</v>
       </c>
       <c r="BG6" s="71">
         <f t="shared" si="1"/>
-        <v>45795</v>
+        <v>45760</v>
       </c>
       <c r="BH6" s="70">
         <f t="shared" si="1"/>
-        <v>45796</v>
+        <v>45761</v>
       </c>
       <c r="BI6" s="62">
         <f t="shared" si="1"/>
-        <v>45797</v>
+        <v>45762</v>
       </c>
       <c r="BJ6" s="62">
         <f t="shared" si="1"/>
-        <v>45798</v>
+        <v>45763</v>
       </c>
       <c r="BK6" s="62">
         <f t="shared" si="1"/>
-        <v>45799</v>
+        <v>45764</v>
       </c>
       <c r="BL6" s="62">
         <f t="shared" si="1"/>
-        <v>45800</v>
+        <v>45765</v>
       </c>
       <c r="BM6" s="62">
         <f t="shared" si="1"/>
-        <v>45801</v>
+        <v>45766</v>
       </c>
       <c r="BN6" s="71">
         <f t="shared" si="1"/>
-        <v>45802</v>
+        <v>45767</v>
       </c>
     </row>
     <row r="7" spans="1:66" s="2" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
@@ -6031,7 +6031,7 @@
         <v>45692</v>
       </c>
       <c r="F10" s="78">
-        <f t="shared" ref="F10:G47" si="6">IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
+        <f t="shared" ref="F10:F46" si="6">IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
         <v>45695</v>
       </c>
       <c r="G10" s="42">
@@ -6775,7 +6775,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="44">
         <f t="shared" si="7"/>
@@ -6861,7 +6861,7 @@
         <v>2</v>
       </c>
       <c r="H20" s="43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="44">
         <f t="shared" si="7"/>
@@ -6946,7 +6946,7 @@
         <v>8</v>
       </c>
       <c r="H21" s="43">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="I21" s="44">
         <f t="shared" si="7"/>
@@ -9775,6 +9775,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="C5:E6"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -9785,15 +9794,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="C5:E6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="H8:H55">
@@ -9899,8 +9899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51EF0A9B-375B-4911-90A2-80351E0CFA76}">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView showGridLines="0" topLeftCell="B24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Débrief de la revue d'avant projet
Compte rendu de la revue, nouvel objectif --> Dossier de financement
</commit_message>
<xml_diff>
--- a/Gestion de Projet/Phase 0/Tableau de bord.xlsx
+++ b/Gestion de Projet/Phase 0/Tableau de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\Documents\Chess-3000\Gestion de Projet\Phase 0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9309EF70-7C23-4231-BDF7-B5564B9E88BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EA0E56-E8AF-4446-86FF-7D0333CED9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3880,6 +3880,9 @@
     <xf numFmtId="1" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3888,22 +3891,19 @@
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="46" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="46" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -5082,9 +5082,9 @@
   </sheetPr>
   <dimension ref="A1:BN56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BO16" sqref="BO16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T24" sqref="T24:AT28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5111,29 +5111,29 @@
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="I1" s="102"/>
-      <c r="K1" s="212" t="s">
+      <c r="K1" s="206" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="212"/>
-      <c r="M1" s="212"/>
-      <c r="N1" s="212"/>
-      <c r="O1" s="212"/>
-      <c r="P1" s="212"/>
-      <c r="Q1" s="212"/>
-      <c r="R1" s="212"/>
-      <c r="S1" s="212"/>
-      <c r="T1" s="212"/>
-      <c r="U1" s="212"/>
-      <c r="V1" s="212"/>
-      <c r="W1" s="212"/>
-      <c r="X1" s="212"/>
-      <c r="Y1" s="212"/>
-      <c r="Z1" s="212"/>
-      <c r="AA1" s="212"/>
-      <c r="AB1" s="212"/>
-      <c r="AC1" s="212"/>
-      <c r="AD1" s="212"/>
-      <c r="AE1" s="212"/>
+      <c r="L1" s="206"/>
+      <c r="M1" s="206"/>
+      <c r="N1" s="206"/>
+      <c r="O1" s="206"/>
+      <c r="P1" s="206"/>
+      <c r="Q1" s="206"/>
+      <c r="R1" s="206"/>
+      <c r="S1" s="206"/>
+      <c r="T1" s="206"/>
+      <c r="U1" s="206"/>
+      <c r="V1" s="206"/>
+      <c r="W1" s="206"/>
+      <c r="X1" s="206"/>
+      <c r="Y1" s="206"/>
+      <c r="Z1" s="206"/>
+      <c r="AA1" s="206"/>
+      <c r="AB1" s="206"/>
+      <c r="AC1" s="206"/>
+      <c r="AD1" s="206"/>
+      <c r="AE1" s="206"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
@@ -5173,11 +5173,11 @@
       <c r="B4" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="213">
+      <c r="C4" s="210">
         <v>45684</v>
       </c>
-      <c r="D4" s="213"/>
-      <c r="E4" s="213"/>
+      <c r="D4" s="210"/>
+      <c r="E4" s="210"/>
       <c r="F4" s="86"/>
       <c r="G4" s="87" t="s">
         <v>73</v>
@@ -5187,86 +5187,86 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="31"/>
-      <c r="K4" s="206" t="str">
+      <c r="K4" s="207" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="L4" s="207"/>
-      <c r="M4" s="207"/>
-      <c r="N4" s="207"/>
-      <c r="O4" s="207"/>
-      <c r="P4" s="207"/>
-      <c r="Q4" s="208"/>
-      <c r="R4" s="206" t="str">
+      <c r="L4" s="208"/>
+      <c r="M4" s="208"/>
+      <c r="N4" s="208"/>
+      <c r="O4" s="208"/>
+      <c r="P4" s="208"/>
+      <c r="Q4" s="209"/>
+      <c r="R4" s="207" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="S4" s="207"/>
-      <c r="T4" s="207"/>
-      <c r="U4" s="207"/>
-      <c r="V4" s="207"/>
-      <c r="W4" s="207"/>
-      <c r="X4" s="208"/>
-      <c r="Y4" s="206" t="str">
+      <c r="S4" s="208"/>
+      <c r="T4" s="208"/>
+      <c r="U4" s="208"/>
+      <c r="V4" s="208"/>
+      <c r="W4" s="208"/>
+      <c r="X4" s="209"/>
+      <c r="Y4" s="207" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="Z4" s="207"/>
-      <c r="AA4" s="207"/>
-      <c r="AB4" s="207"/>
-      <c r="AC4" s="207"/>
-      <c r="AD4" s="207"/>
-      <c r="AE4" s="208"/>
-      <c r="AF4" s="206" t="str">
+      <c r="Z4" s="208"/>
+      <c r="AA4" s="208"/>
+      <c r="AB4" s="208"/>
+      <c r="AC4" s="208"/>
+      <c r="AD4" s="208"/>
+      <c r="AE4" s="209"/>
+      <c r="AF4" s="207" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="AG4" s="207"/>
-      <c r="AH4" s="207"/>
-      <c r="AI4" s="207"/>
-      <c r="AJ4" s="207"/>
-      <c r="AK4" s="207"/>
-      <c r="AL4" s="208"/>
-      <c r="AM4" s="206" t="str">
+      <c r="AG4" s="208"/>
+      <c r="AH4" s="208"/>
+      <c r="AI4" s="208"/>
+      <c r="AJ4" s="208"/>
+      <c r="AK4" s="208"/>
+      <c r="AL4" s="209"/>
+      <c r="AM4" s="207" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="AN4" s="207"/>
-      <c r="AO4" s="207"/>
-      <c r="AP4" s="207"/>
-      <c r="AQ4" s="207"/>
-      <c r="AR4" s="207"/>
-      <c r="AS4" s="208"/>
-      <c r="AT4" s="206" t="str">
+      <c r="AN4" s="208"/>
+      <c r="AO4" s="208"/>
+      <c r="AP4" s="208"/>
+      <c r="AQ4" s="208"/>
+      <c r="AR4" s="208"/>
+      <c r="AS4" s="209"/>
+      <c r="AT4" s="207" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="AU4" s="207"/>
-      <c r="AV4" s="207"/>
-      <c r="AW4" s="207"/>
-      <c r="AX4" s="207"/>
-      <c r="AY4" s="207"/>
-      <c r="AZ4" s="208"/>
-      <c r="BA4" s="206" t="str">
+      <c r="AU4" s="208"/>
+      <c r="AV4" s="208"/>
+      <c r="AW4" s="208"/>
+      <c r="AX4" s="208"/>
+      <c r="AY4" s="208"/>
+      <c r="AZ4" s="209"/>
+      <c r="BA4" s="207" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="BB4" s="207"/>
-      <c r="BC4" s="207"/>
-      <c r="BD4" s="207"/>
-      <c r="BE4" s="207"/>
-      <c r="BF4" s="207"/>
-      <c r="BG4" s="208"/>
-      <c r="BH4" s="206" t="str">
+      <c r="BB4" s="208"/>
+      <c r="BC4" s="208"/>
+      <c r="BD4" s="208"/>
+      <c r="BE4" s="208"/>
+      <c r="BF4" s="208"/>
+      <c r="BG4" s="209"/>
+      <c r="BH4" s="207" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="BI4" s="207"/>
-      <c r="BJ4" s="207"/>
-      <c r="BK4" s="207"/>
-      <c r="BL4" s="207"/>
-      <c r="BM4" s="207"/>
-      <c r="BN4" s="208"/>
+      <c r="BI4" s="208"/>
+      <c r="BJ4" s="208"/>
+      <c r="BK4" s="208"/>
+      <c r="BL4" s="208"/>
+      <c r="BM4" s="208"/>
+      <c r="BN4" s="209"/>
     </row>
     <row r="5" spans="1:66" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
@@ -5283,86 +5283,86 @@
       <c r="H5" s="86"/>
       <c r="I5" s="86"/>
       <c r="J5" s="31"/>
-      <c r="K5" s="209">
+      <c r="K5" s="211">
         <f>K6</f>
         <v>45712</v>
       </c>
-      <c r="L5" s="210"/>
-      <c r="M5" s="210"/>
-      <c r="N5" s="210"/>
-      <c r="O5" s="210"/>
-      <c r="P5" s="210"/>
-      <c r="Q5" s="211"/>
-      <c r="R5" s="209">
+      <c r="L5" s="212"/>
+      <c r="M5" s="212"/>
+      <c r="N5" s="212"/>
+      <c r="O5" s="212"/>
+      <c r="P5" s="212"/>
+      <c r="Q5" s="213"/>
+      <c r="R5" s="211">
         <f>R6</f>
         <v>45719</v>
       </c>
-      <c r="S5" s="210"/>
-      <c r="T5" s="210"/>
-      <c r="U5" s="210"/>
-      <c r="V5" s="210"/>
-      <c r="W5" s="210"/>
-      <c r="X5" s="211"/>
-      <c r="Y5" s="209">
+      <c r="S5" s="212"/>
+      <c r="T5" s="212"/>
+      <c r="U5" s="212"/>
+      <c r="V5" s="212"/>
+      <c r="W5" s="212"/>
+      <c r="X5" s="213"/>
+      <c r="Y5" s="211">
         <f>Y6</f>
         <v>45726</v>
       </c>
-      <c r="Z5" s="210"/>
-      <c r="AA5" s="210"/>
-      <c r="AB5" s="210"/>
-      <c r="AC5" s="210"/>
-      <c r="AD5" s="210"/>
-      <c r="AE5" s="211"/>
-      <c r="AF5" s="209">
+      <c r="Z5" s="212"/>
+      <c r="AA5" s="212"/>
+      <c r="AB5" s="212"/>
+      <c r="AC5" s="212"/>
+      <c r="AD5" s="212"/>
+      <c r="AE5" s="213"/>
+      <c r="AF5" s="211">
         <f>AF6</f>
         <v>45733</v>
       </c>
-      <c r="AG5" s="210"/>
-      <c r="AH5" s="210"/>
-      <c r="AI5" s="210"/>
-      <c r="AJ5" s="210"/>
-      <c r="AK5" s="210"/>
-      <c r="AL5" s="211"/>
-      <c r="AM5" s="209">
+      <c r="AG5" s="212"/>
+      <c r="AH5" s="212"/>
+      <c r="AI5" s="212"/>
+      <c r="AJ5" s="212"/>
+      <c r="AK5" s="212"/>
+      <c r="AL5" s="213"/>
+      <c r="AM5" s="211">
         <f>AM6</f>
         <v>45740</v>
       </c>
-      <c r="AN5" s="210"/>
-      <c r="AO5" s="210"/>
-      <c r="AP5" s="210"/>
-      <c r="AQ5" s="210"/>
-      <c r="AR5" s="210"/>
-      <c r="AS5" s="211"/>
-      <c r="AT5" s="209">
+      <c r="AN5" s="212"/>
+      <c r="AO5" s="212"/>
+      <c r="AP5" s="212"/>
+      <c r="AQ5" s="212"/>
+      <c r="AR5" s="212"/>
+      <c r="AS5" s="213"/>
+      <c r="AT5" s="211">
         <f>AT6</f>
         <v>45747</v>
       </c>
-      <c r="AU5" s="210"/>
-      <c r="AV5" s="210"/>
-      <c r="AW5" s="210"/>
-      <c r="AX5" s="210"/>
-      <c r="AY5" s="210"/>
-      <c r="AZ5" s="211"/>
-      <c r="BA5" s="209">
+      <c r="AU5" s="212"/>
+      <c r="AV5" s="212"/>
+      <c r="AW5" s="212"/>
+      <c r="AX5" s="212"/>
+      <c r="AY5" s="212"/>
+      <c r="AZ5" s="213"/>
+      <c r="BA5" s="211">
         <f>BA6</f>
         <v>45754</v>
       </c>
-      <c r="BB5" s="210"/>
-      <c r="BC5" s="210"/>
-      <c r="BD5" s="210"/>
-      <c r="BE5" s="210"/>
-      <c r="BF5" s="210"/>
-      <c r="BG5" s="211"/>
-      <c r="BH5" s="209">
+      <c r="BB5" s="212"/>
+      <c r="BC5" s="212"/>
+      <c r="BD5" s="212"/>
+      <c r="BE5" s="212"/>
+      <c r="BF5" s="212"/>
+      <c r="BG5" s="213"/>
+      <c r="BH5" s="211">
         <f>BH6</f>
         <v>45761</v>
       </c>
-      <c r="BI5" s="210"/>
-      <c r="BJ5" s="210"/>
-      <c r="BK5" s="210"/>
-      <c r="BL5" s="210"/>
-      <c r="BM5" s="210"/>
-      <c r="BN5" s="211"/>
+      <c r="BI5" s="212"/>
+      <c r="BJ5" s="212"/>
+      <c r="BK5" s="212"/>
+      <c r="BL5" s="212"/>
+      <c r="BM5" s="212"/>
+      <c r="BN5" s="213"/>
     </row>
     <row r="6" spans="1:66" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
@@ -7163,7 +7163,7 @@
       <c r="BM23" s="40"/>
       <c r="BN23" s="40"/>
     </row>
-    <row r="24" spans="1:66" s="41" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:66" s="41" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>2.1.1</v>
@@ -9775,15 +9775,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="C5:E6"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -9794,6 +9785,15 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="C5:E6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="H8:H55">

</xml_diff>